<commit_message>
change data comite de tumors
</commit_message>
<xml_diff>
--- a/register/completedRegister.xlsx
+++ b/register/completedRegister.xlsx
@@ -379,7 +379,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BD50"/>
+  <dimension ref="A1:BD52"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -7699,9 +7699,337 @@
         <v>43495</v>
       </c>
     </row>
+    <row r="51">
+      <c r="A51" s="1" t="str">
+        <v>Resecció/ns limitada/es</v>
+      </c>
+      <c r="B51" s="1">
+        <v>1674</v>
+      </c>
+      <c r="C51" s="1">
+        <v>1532</v>
+      </c>
+      <c r="D51" s="1" t="str">
+        <v>Josep</v>
+      </c>
+      <c r="E51" s="1" t="str">
+        <v>Bros</v>
+      </c>
+      <c r="F51" s="1" t="str">
+        <v>Bros</v>
+      </c>
+      <c r="G51" s="1">
+        <v>16221522</v>
+      </c>
+      <c r="H51" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="I51" s="1" t="str">
+        <v>Home</v>
+      </c>
+      <c r="J51" s="1" t="str">
+        <v>64</v>
+      </c>
+      <c r="K51" s="1" t="str">
+        <v>83</v>
+      </c>
+      <c r="L51" s="1">
+        <v>177</v>
+      </c>
+      <c r="M51" s="1">
+        <v>27</v>
+      </c>
+      <c r="N51" s="1">
+        <v>2</v>
+      </c>
+      <c r="O51" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="P51" s="2">
+        <v>43699</v>
+      </c>
+      <c r="Q51" s="1" t="str">
+        <v>Resecció Menor (&lt;3 segm)</v>
+      </c>
+      <c r="R51" s="1" t="str">
+        <v>reseccio del caudat, tres enucleacions i una RF</v>
+      </c>
+      <c r="S51" s="1" t="str">
+        <v>Oberta</v>
+      </c>
+      <c r="T51" s="1" t="str">
+        <v>Si, simultània amb la hepatectomia</v>
+      </c>
+      <c r="U51" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="V51" s="1" t="str">
+        <v>Impressió R1</v>
+      </c>
+      <c r="W51" s="1">
+        <v>4</v>
+      </c>
+      <c r="X51" s="1">
+        <v>2</v>
+      </c>
+      <c r="Y51" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="Z51" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AA51" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AB51" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AC51" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AD51" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AE51" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AF51" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AH51" s="1">
+        <v>4</v>
+      </c>
+      <c r="AI51" s="1">
+        <v>2.7</v>
+      </c>
+      <c r="AJ51" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK51" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AL51" s="1" t="str">
+        <v>aquamantis a totes les reseccions</v>
+      </c>
+      <c r="AM51" s="2">
+        <v>44022</v>
+      </c>
+      <c r="AN51" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AO51" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AP51" s="1" t="str">
+        <v>Viu</v>
+      </c>
+      <c r="AQ51" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AR51" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AS51" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AT51" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AU51" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AV51" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AW51" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AX51" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AY51" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AZ51" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="BA51" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BC51" s="2">
+        <v>44605.694823854166</v>
+      </c>
+      <c r="BD51" s="2">
+        <v>43495</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="str">
+        <v>Resecció/ns limitada/es</v>
+      </c>
+      <c r="B52" s="1">
+        <v>1674</v>
+      </c>
+      <c r="C52" s="1">
+        <v>1532</v>
+      </c>
+      <c r="D52" s="1" t="str">
+        <v>Josep</v>
+      </c>
+      <c r="E52" s="1" t="str">
+        <v>Bros</v>
+      </c>
+      <c r="F52" s="1" t="str">
+        <v>Bros</v>
+      </c>
+      <c r="G52" s="1">
+        <v>16221522</v>
+      </c>
+      <c r="H52" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="I52" s="1" t="str">
+        <v>Home</v>
+      </c>
+      <c r="J52" s="1" t="str">
+        <v>64</v>
+      </c>
+      <c r="K52" s="1" t="str">
+        <v>83</v>
+      </c>
+      <c r="L52" s="1">
+        <v>177</v>
+      </c>
+      <c r="M52" s="1">
+        <v>27</v>
+      </c>
+      <c r="N52" s="1">
+        <v>2</v>
+      </c>
+      <c r="O52" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="P52" s="2">
+        <v>43699</v>
+      </c>
+      <c r="Q52" s="1" t="str">
+        <v>Resecció Menor (&lt;3 segm)</v>
+      </c>
+      <c r="R52" s="1" t="str">
+        <v>reseccio del caudat, tres enucleacions i una RF</v>
+      </c>
+      <c r="S52" s="1" t="str">
+        <v>Oberta</v>
+      </c>
+      <c r="T52" s="1" t="str">
+        <v>Si, simultània amb la hepatectomia</v>
+      </c>
+      <c r="U52" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="V52" s="1" t="str">
+        <v>Impressió R1</v>
+      </c>
+      <c r="W52" s="1">
+        <v>4</v>
+      </c>
+      <c r="X52" s="1">
+        <v>2</v>
+      </c>
+      <c r="Y52" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="Z52" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AA52" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AB52" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AC52" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AD52" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AE52" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AF52" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AH52" s="1">
+        <v>4</v>
+      </c>
+      <c r="AI52" s="1">
+        <v>2.7</v>
+      </c>
+      <c r="AJ52" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK52" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AL52" s="1" t="str">
+        <v>aquamantis a totes les reseccions</v>
+      </c>
+      <c r="AM52" s="2">
+        <v>44022</v>
+      </c>
+      <c r="AN52" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AO52" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AP52" s="1" t="str">
+        <v>Viu</v>
+      </c>
+      <c r="AQ52" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AR52" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AS52" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AT52" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AU52" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AV52" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AW52" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AX52" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AY52" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AZ52" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="BA52" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BC52" s="2">
+        <v>44605.69677539352</v>
+      </c>
+      <c r="BD52" s="2">
+        <v>43495</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:BD50"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:BD52"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add clavien dindo calculator
</commit_message>
<xml_diff>
--- a/register/completedRegister.xlsx
+++ b/register/completedRegister.xlsx
@@ -379,7 +379,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BD52"/>
+  <dimension ref="A1:BD53"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -8027,9 +8027,173 @@
         <v>43495</v>
       </c>
     </row>
+    <row r="53">
+      <c r="A53" s="1" t="str">
+        <v>Resecció/ns limitada/es</v>
+      </c>
+      <c r="B53" s="1">
+        <v>1674</v>
+      </c>
+      <c r="C53" s="1">
+        <v>1532</v>
+      </c>
+      <c r="D53" s="1" t="str">
+        <v>Josep</v>
+      </c>
+      <c r="E53" s="1" t="str">
+        <v>Bros</v>
+      </c>
+      <c r="F53" s="1" t="str">
+        <v>Bros</v>
+      </c>
+      <c r="G53" s="1">
+        <v>16221522</v>
+      </c>
+      <c r="H53" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="I53" s="1" t="str">
+        <v>Home</v>
+      </c>
+      <c r="J53" s="1" t="str">
+        <v>64</v>
+      </c>
+      <c r="K53" s="1" t="str">
+        <v>83</v>
+      </c>
+      <c r="L53" s="1">
+        <v>177</v>
+      </c>
+      <c r="M53" s="1">
+        <v>27</v>
+      </c>
+      <c r="N53" s="1">
+        <v>2</v>
+      </c>
+      <c r="O53" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="P53" s="2">
+        <v>43699</v>
+      </c>
+      <c r="Q53" s="1" t="str">
+        <v>Resecció Menor (&lt;3 segm)</v>
+      </c>
+      <c r="R53" s="1" t="str">
+        <v>reseccio del caudat, tres enucleacions i una RF</v>
+      </c>
+      <c r="S53" s="1" t="str">
+        <v>Oberta</v>
+      </c>
+      <c r="T53" s="1" t="str">
+        <v>Si, simultània amb la hepatectomia</v>
+      </c>
+      <c r="U53" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="V53" s="1" t="str">
+        <v>Impressió R1</v>
+      </c>
+      <c r="W53" s="1">
+        <v>4</v>
+      </c>
+      <c r="X53" s="1">
+        <v>2</v>
+      </c>
+      <c r="Y53" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="Z53" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AA53" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AB53" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AC53" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AD53" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AE53" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AF53" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AH53" s="1">
+        <v>4</v>
+      </c>
+      <c r="AI53" s="1">
+        <v>2.7</v>
+      </c>
+      <c r="AJ53" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK53" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AL53" s="1" t="str">
+        <v>aquamantis a totes les reseccions</v>
+      </c>
+      <c r="AM53" s="2">
+        <v>44022</v>
+      </c>
+      <c r="AN53" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AO53" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AP53" s="1" t="str">
+        <v>Viu</v>
+      </c>
+      <c r="AQ53" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AR53" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AS53" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AT53" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AU53" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AV53" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AW53" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AX53" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AY53" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AZ53" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="BA53" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BC53" s="2">
+        <v>44605.75277976852</v>
+      </c>
+      <c r="BD53" s="2">
+        <v>43495</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:BD52"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:BD53"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
correct some inputs and clavien
</commit_message>
<xml_diff>
--- a/register/completedRegister.xlsx
+++ b/register/completedRegister.xlsx
@@ -379,7 +379,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BF16"/>
+  <dimension ref="A1:BH31"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -559,6 +559,12 @@
       <c r="BF1" s="1" t="str">
         <v>TIPUS CIRCOLONSIM</v>
       </c>
+      <c r="BG1" s="1" t="str">
+        <v>Causa REIQ</v>
+      </c>
+      <c r="BH1" s="1" t="str">
+        <v>GRAU FB</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="str">
@@ -3059,18 +3065,2505 @@
         <v>26</v>
       </c>
       <c r="BB16" s="2">
-        <v>44607.92932018518</v>
+        <v>44607.92932016204</v>
       </c>
       <c r="BC16" s="2">
         <v>43416</v>
       </c>
       <c r="BD16" s="1" t="str">
         <v>No</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="str">
+        <v>Resecció/ns limitada/es</v>
+      </c>
+      <c r="B17" s="1">
+        <v>1693</v>
+      </c>
+      <c r="C17" s="1" t="str">
+        <v>14/06/2019</v>
+      </c>
+      <c r="D17" s="1" t="str">
+        <v>24/07/2020</v>
+      </c>
+      <c r="E17" s="1" t="str">
+        <v>23/05/2019</v>
+      </c>
+      <c r="F17" s="1" t="str">
+        <v>IV,VII,VI,VIII</v>
+      </c>
+      <c r="G17" s="1">
+        <v>1547</v>
+      </c>
+      <c r="H17" s="1" t="str">
+        <v>Josep</v>
+      </c>
+      <c r="I17" s="1" t="str">
+        <v>Moline</v>
+      </c>
+      <c r="J17" s="1" t="str">
+        <v>Masana</v>
+      </c>
+      <c r="K17" s="1">
+        <v>16384162</v>
+      </c>
+      <c r="L17" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="M17" s="1" t="str">
+        <v>Home</v>
+      </c>
+      <c r="N17" s="1" t="str">
+        <v>69</v>
+      </c>
+      <c r="O17" s="1" t="str">
+        <v>100</v>
+      </c>
+      <c r="P17" s="1">
+        <v>180</v>
+      </c>
+      <c r="Q17" s="1">
+        <v>29</v>
+      </c>
+      <c r="R17" s="1">
+        <v>3</v>
+      </c>
+      <c r="S17" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="T17" s="2">
+        <v>43812</v>
+      </c>
+      <c r="U17" s="1" t="str">
+        <v>Resecció Menor (&lt;3 segm)</v>
+      </c>
+      <c r="V17" s="1" t="str">
+        <v>segmentect 4b + tres RL, una al cavocava dret</v>
+      </c>
+      <c r="W17" s="1" t="str">
+        <v>Oberta</v>
+      </c>
+      <c r="X17" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="Y17" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="Z17" s="1" t="str">
+        <v>Impressió R0</v>
+      </c>
+      <c r="AA17" s="1">
+        <v>4</v>
+      </c>
+      <c r="AB17" s="1">
+        <v>3</v>
+      </c>
+      <c r="AC17" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AD17" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AE17" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AF17" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AG17" s="1" t="str">
+        <v>I</v>
+      </c>
+      <c r="AH17" s="1">
+        <v>9</v>
+      </c>
+      <c r="AI17" s="1">
+        <v>4</v>
+      </c>
+      <c r="AJ17" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="AK17" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL17" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AM17" s="1" t="str">
+        <v>VSD</v>
+      </c>
+      <c r="AN17" s="2">
+        <v>43984</v>
+      </c>
+      <c r="AO17" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AP17" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AQ17" s="1" t="str">
+        <v>Viu</v>
+      </c>
+      <c r="AR17" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AS17" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AT17" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AU17" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AV17" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AW17" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AX17" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AY17" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AZ17" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BA17" s="1">
+        <v>10</v>
+      </c>
+      <c r="BB17" s="2">
+        <v>44608.35907756945</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="str">
+        <v>Hepatectomia major + resecció contralateral</v>
+      </c>
+      <c r="B18" s="1">
+        <v>1687</v>
+      </c>
+      <c r="C18" s="1" t="str">
+        <v>17/05/2019</v>
+      </c>
+      <c r="D18" s="1" t="str">
+        <v>26/07/2019</v>
+      </c>
+      <c r="E18" s="1" t="str">
+        <v>22/03/2019</v>
+      </c>
+      <c r="F18" s="1" t="str">
+        <v>III,II,VIII,V,IV</v>
+      </c>
+      <c r="G18" s="1">
+        <v>1543</v>
+      </c>
+      <c r="H18" s="1" t="str">
+        <v>Tomas</v>
+      </c>
+      <c r="I18" s="1" t="str">
+        <v>Mata</v>
+      </c>
+      <c r="J18" s="1" t="str">
+        <v>Beltran</v>
+      </c>
+      <c r="K18" s="1">
+        <v>13109704</v>
+      </c>
+      <c r="L18" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="M18" s="1" t="str">
+        <v>Home</v>
+      </c>
+      <c r="N18" s="1" t="str">
+        <v>83</v>
+      </c>
+      <c r="O18" s="1" t="str">
+        <v>68</v>
+      </c>
+      <c r="P18" s="1">
+        <v>160</v>
+      </c>
+      <c r="Q18" s="1">
+        <v>26</v>
+      </c>
+      <c r="R18" s="1">
+        <v>3</v>
+      </c>
+      <c r="S18" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="T18" s="2">
+        <v>43784</v>
+      </c>
+      <c r="U18" s="1" t="str">
+        <v>Resecció Major (&gt;= 3 segm)</v>
+      </c>
+      <c r="V18" s="1" t="str">
+        <v>Hepatect esqu i RL 8 i RF 5</v>
+      </c>
+      <c r="W18" s="1" t="str">
+        <v>Oberta</v>
+      </c>
+      <c r="X18" s="1" t="str">
+        <v>Si, simultània amb la hepatectomia</v>
+      </c>
+      <c r="Y18" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="Z18" s="1" t="str">
+        <v>Impressió R0</v>
+      </c>
+      <c r="AA18" s="1">
+        <v>5</v>
+      </c>
+      <c r="AB18" s="1">
+        <v>2</v>
+      </c>
+      <c r="AC18" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AE18" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AF18" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AG18" s="1" t="str">
+        <v>0</v>
+      </c>
+      <c r="AH18" s="1">
+        <v>0</v>
+      </c>
+      <c r="AI18" s="1">
+        <v>3</v>
+      </c>
+      <c r="AJ18" s="1">
+        <v>3</v>
+      </c>
+      <c r="AK18" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="AL18" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AN18" s="2">
+        <v>44077</v>
+      </c>
+      <c r="AO18" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AP18" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AQ18" s="1" t="str">
+        <v>Viu</v>
+      </c>
+      <c r="AR18" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AS18" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AT18" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AU18" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AV18" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AW18" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AX18" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BB18" s="2">
+        <v>44608.36407142361</v>
+      </c>
+      <c r="BC18" s="2">
+        <v>43621</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="str">
+        <v>Hepatectomia dreta</v>
+      </c>
+      <c r="B19" s="1">
+        <v>1695</v>
+      </c>
+      <c r="C19" s="1" t="str">
+        <v>09/07/2018</v>
+      </c>
+      <c r="D19" s="1" t="str">
+        <v>11/02/2019</v>
+      </c>
+      <c r="E19" s="1" t="str">
+        <v>25/06/2018</v>
+      </c>
+      <c r="F19" s="1" t="str">
+        <v>VII</v>
+      </c>
+      <c r="H19" s="1" t="str">
+        <v>Jordi</v>
+      </c>
+      <c r="I19" s="1" t="str">
+        <v>Morillas2</v>
+      </c>
+      <c r="J19" s="1" t="str">
+        <v>Esteban2</v>
+      </c>
+      <c r="K19" s="1">
+        <v>13296015</v>
+      </c>
+      <c r="L19" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="O19" s="1" t="str">
+        <v>79</v>
+      </c>
+      <c r="P19" s="1">
+        <v>178</v>
+      </c>
+      <c r="Q19" s="1">
+        <v>25</v>
+      </c>
+      <c r="R19" s="1">
+        <v>3</v>
+      </c>
+      <c r="S19" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="T19" s="2">
+        <v>43858</v>
+      </c>
+      <c r="U19" s="1" t="str">
+        <v>Resecció Major (&gt;= 3 segm)</v>
+      </c>
+      <c r="V19" s="1" t="str">
+        <v>hepatectomia dreta</v>
+      </c>
+      <c r="W19" s="1" t="str">
+        <v>Oberta</v>
+      </c>
+      <c r="X19" s="1" t="str">
+        <v>Si, com a primer temps quirúrgic</v>
+      </c>
+      <c r="Y19" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="Z19" s="1" t="str">
+        <v>Impressió R1</v>
+      </c>
+      <c r="AA19" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB19" s="1">
+        <v>3</v>
+      </c>
+      <c r="AC19" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AD19" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AE19" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AF19" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AG19" s="1" t="str">
+        <v>IIIb</v>
+      </c>
+      <c r="AH19" s="1">
+        <v>61</v>
+      </c>
+      <c r="AI19" s="1">
+        <v>1</v>
+      </c>
+      <c r="AJ19" s="1">
+        <v>3</v>
+      </c>
+      <c r="AK19" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL19" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AM19" s="1" t="str">
+        <v>ampliacio quirurgica</v>
+      </c>
+      <c r="AN19" s="2">
+        <v>43983</v>
+      </c>
+      <c r="AO19" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AP19" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AQ19" s="1" t="str">
+        <v>Viu</v>
+      </c>
+      <c r="AR19" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AS19" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AT19" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AU19" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AV19" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AW19" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AX19" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AY19" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AZ19" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BA19" s="1">
+        <v>55</v>
+      </c>
+      <c r="BB19" s="2">
+        <v>44608.36987771991</v>
+      </c>
+      <c r="BC19" s="2">
+        <v>43446</v>
+      </c>
+      <c r="BD19" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BG19" s="1" t="str">
+        <v>oclusió, peritonitis fecaoidea</v>
+      </c>
+      <c r="BH19" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="str">
+        <v>Hepatectomia dreta</v>
+      </c>
+      <c r="B20" s="1">
+        <v>1695</v>
+      </c>
+      <c r="C20" s="1" t="str">
+        <v>09/07/2018</v>
+      </c>
+      <c r="D20" s="1" t="str">
+        <v>11/02/2019</v>
+      </c>
+      <c r="E20" s="1" t="str">
+        <v>25/06/2018</v>
+      </c>
+      <c r="F20" s="1" t="str">
+        <v>VII</v>
+      </c>
+      <c r="H20" s="1" t="str">
+        <v>Jordi</v>
+      </c>
+      <c r="I20" s="1" t="str">
+        <v>Morillas2</v>
+      </c>
+      <c r="J20" s="1" t="str">
+        <v>Esteban2</v>
+      </c>
+      <c r="K20" s="1">
+        <v>13296015</v>
+      </c>
+      <c r="L20" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="O20" s="1" t="str">
+        <v>79</v>
+      </c>
+      <c r="P20" s="1">
+        <v>178</v>
+      </c>
+      <c r="Q20" s="1">
+        <v>25</v>
+      </c>
+      <c r="R20" s="1">
+        <v>3</v>
+      </c>
+      <c r="S20" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="T20" s="2">
+        <v>43858</v>
+      </c>
+      <c r="U20" s="1" t="str">
+        <v>Resecció Major (&gt;= 3 segm)</v>
+      </c>
+      <c r="V20" s="1" t="str">
+        <v>hepatectomia dreta</v>
+      </c>
+      <c r="W20" s="1" t="str">
+        <v>Oberta</v>
+      </c>
+      <c r="X20" s="1" t="str">
+        <v>Si, com a primer temps quirúrgic</v>
+      </c>
+      <c r="Y20" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="Z20" s="1" t="str">
+        <v>Impressió R1</v>
+      </c>
+      <c r="AA20" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB20" s="1">
+        <v>3</v>
+      </c>
+      <c r="AC20" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AD20" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AE20" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AF20" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AG20" s="1" t="str">
+        <v>IIIb</v>
+      </c>
+      <c r="AH20" s="1">
+        <v>61</v>
+      </c>
+      <c r="AI20" s="1">
+        <v>1</v>
+      </c>
+      <c r="AJ20" s="1">
+        <v>3</v>
+      </c>
+      <c r="AK20" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL20" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AM20" s="1" t="str">
+        <v>ampliacio quirurgica</v>
+      </c>
+      <c r="AN20" s="2">
+        <v>43983</v>
+      </c>
+      <c r="AO20" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AP20" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AQ20" s="1" t="str">
+        <v>Viu</v>
+      </c>
+      <c r="AR20" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AS20" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AT20" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AU20" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AV20" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AW20" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AX20" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AY20" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AZ20" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BA20" s="1">
+        <v>55</v>
+      </c>
+      <c r="BB20" s="2">
+        <v>44608.37466033565</v>
+      </c>
+      <c r="BC20" s="2">
+        <v>43446</v>
+      </c>
+      <c r="BD20" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BG20" s="1" t="str">
+        <v>oclusió, peritonitis fecaoidea</v>
+      </c>
+      <c r="BH20" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="str">
+        <v>Hepatectomia dreta</v>
+      </c>
+      <c r="B21" s="1">
+        <v>1695</v>
+      </c>
+      <c r="C21" s="1" t="str">
+        <v>09/07/2018</v>
+      </c>
+      <c r="D21" s="1" t="str">
+        <v>11/02/2019</v>
+      </c>
+      <c r="E21" s="1" t="str">
+        <v>25/06/2018</v>
+      </c>
+      <c r="F21" s="1" t="str">
+        <v>VII</v>
+      </c>
+      <c r="H21" s="1" t="str">
+        <v>Jordi</v>
+      </c>
+      <c r="I21" s="1" t="str">
+        <v>Morillas2</v>
+      </c>
+      <c r="J21" s="1" t="str">
+        <v>Esteban2</v>
+      </c>
+      <c r="K21" s="1">
+        <v>13296015</v>
+      </c>
+      <c r="L21" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="O21" s="1" t="str">
+        <v>79</v>
+      </c>
+      <c r="P21" s="1">
+        <v>178</v>
+      </c>
+      <c r="Q21" s="1">
+        <v>25</v>
+      </c>
+      <c r="R21" s="1">
+        <v>3</v>
+      </c>
+      <c r="S21" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="T21" s="2">
+        <v>43858</v>
+      </c>
+      <c r="U21" s="1" t="str">
+        <v>Resecció Major (&gt;= 3 segm)</v>
+      </c>
+      <c r="V21" s="1" t="str">
+        <v>hepatectomia dreta</v>
+      </c>
+      <c r="W21" s="1" t="str">
+        <v>Oberta</v>
+      </c>
+      <c r="X21" s="1" t="str">
+        <v>Si, com a primer temps quirúrgic</v>
+      </c>
+      <c r="Y21" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="Z21" s="1" t="str">
+        <v>Impressió R1</v>
+      </c>
+      <c r="AA21" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB21" s="1">
+        <v>3</v>
+      </c>
+      <c r="AC21" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AD21" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AE21" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AF21" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AG21" s="1" t="str">
+        <v>IIIb</v>
+      </c>
+      <c r="AH21" s="1">
+        <v>61</v>
+      </c>
+      <c r="AI21" s="1">
+        <v>1</v>
+      </c>
+      <c r="AJ21" s="1">
+        <v>3</v>
+      </c>
+      <c r="AK21" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL21" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AM21" s="1" t="str">
+        <v>ampliacio quirurgica</v>
+      </c>
+      <c r="AN21" s="2">
+        <v>43983</v>
+      </c>
+      <c r="AO21" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AP21" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AQ21" s="1" t="str">
+        <v>Viu</v>
+      </c>
+      <c r="AR21" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AS21" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AT21" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AU21" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AV21" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AW21" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AX21" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AY21" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AZ21" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BA21" s="1">
+        <v>55</v>
+      </c>
+      <c r="BB21" s="2">
+        <v>44608.37611074074</v>
+      </c>
+      <c r="BC21" s="2">
+        <v>43446</v>
+      </c>
+      <c r="BD21" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BG21" s="1" t="str">
+        <v>oclusió, peritonitis fecaoidea</v>
+      </c>
+      <c r="BH21" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="str">
+        <v>Hepatectomia dreta</v>
+      </c>
+      <c r="B22" s="1">
+        <v>1695</v>
+      </c>
+      <c r="C22" s="1" t="str">
+        <v>09/07/2018</v>
+      </c>
+      <c r="D22" s="1" t="str">
+        <v>11/02/2019</v>
+      </c>
+      <c r="E22" s="1" t="str">
+        <v>25/06/2018</v>
+      </c>
+      <c r="F22" s="1" t="str">
+        <v>VII</v>
+      </c>
+      <c r="H22" s="1" t="str">
+        <v>Jordi</v>
+      </c>
+      <c r="I22" s="1" t="str">
+        <v>Morillas2</v>
+      </c>
+      <c r="J22" s="1" t="str">
+        <v>Esteban2</v>
+      </c>
+      <c r="K22" s="1">
+        <v>13296015</v>
+      </c>
+      <c r="L22" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="O22" s="1" t="str">
+        <v>79</v>
+      </c>
+      <c r="P22" s="1">
+        <v>178</v>
+      </c>
+      <c r="Q22" s="1">
+        <v>25</v>
+      </c>
+      <c r="R22" s="1">
+        <v>3</v>
+      </c>
+      <c r="S22" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="T22" s="2">
+        <v>43858</v>
+      </c>
+      <c r="U22" s="1" t="str">
+        <v>Resecció Major (&gt;= 3 segm)</v>
+      </c>
+      <c r="V22" s="1" t="str">
+        <v>hepatectomia dreta</v>
+      </c>
+      <c r="W22" s="1" t="str">
+        <v>Oberta</v>
+      </c>
+      <c r="X22" s="1" t="str">
+        <v>Si, com a primer temps quirúrgic</v>
+      </c>
+      <c r="Y22" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="Z22" s="1" t="str">
+        <v>Impressió R1</v>
+      </c>
+      <c r="AA22" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB22" s="1">
+        <v>3</v>
+      </c>
+      <c r="AC22" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AD22" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AE22" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AF22" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AG22" s="1" t="str">
+        <v>IIIb</v>
+      </c>
+      <c r="AH22" s="1">
+        <v>61</v>
+      </c>
+      <c r="AI22" s="1">
+        <v>1</v>
+      </c>
+      <c r="AJ22" s="1">
+        <v>3</v>
+      </c>
+      <c r="AK22" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL22" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AM22" s="1" t="str">
+        <v>ampliacio quirurgica</v>
+      </c>
+      <c r="AN22" s="2">
+        <v>43983</v>
+      </c>
+      <c r="AO22" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AP22" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AQ22" s="1" t="str">
+        <v>Viu</v>
+      </c>
+      <c r="AR22" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AS22" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AT22" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AU22" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AV22" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AW22" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AX22" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AY22" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AZ22" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BA22" s="1">
+        <v>55</v>
+      </c>
+      <c r="BB22" s="2">
+        <v>44608.37847253472</v>
+      </c>
+      <c r="BC22" s="2">
+        <v>43446</v>
+      </c>
+      <c r="BD22" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BG22" s="1" t="str">
+        <v>oclusió, peritonitis fecaoidea</v>
+      </c>
+      <c r="BH22" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="str">
+        <v>Hepatectomia dreta</v>
+      </c>
+      <c r="B23" s="1">
+        <v>1695</v>
+      </c>
+      <c r="C23" s="1" t="str">
+        <v>09/07/2018</v>
+      </c>
+      <c r="D23" s="1" t="str">
+        <v>11/02/2019</v>
+      </c>
+      <c r="E23" s="1" t="str">
+        <v>25/06/2018</v>
+      </c>
+      <c r="F23" s="1" t="str">
+        <v>VII</v>
+      </c>
+      <c r="H23" s="1" t="str">
+        <v>Jordi</v>
+      </c>
+      <c r="I23" s="1" t="str">
+        <v>Morillas2</v>
+      </c>
+      <c r="J23" s="1" t="str">
+        <v>Esteban2</v>
+      </c>
+      <c r="K23" s="1">
+        <v>13296015</v>
+      </c>
+      <c r="L23" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="O23" s="1" t="str">
+        <v>79</v>
+      </c>
+      <c r="P23" s="1">
+        <v>178</v>
+      </c>
+      <c r="Q23" s="1">
+        <v>25</v>
+      </c>
+      <c r="R23" s="1">
+        <v>3</v>
+      </c>
+      <c r="S23" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="T23" s="2">
+        <v>43858</v>
+      </c>
+      <c r="U23" s="1" t="str">
+        <v>Resecció Major (&gt;= 3 segm)</v>
+      </c>
+      <c r="V23" s="1" t="str">
+        <v>hepatectomia dreta</v>
+      </c>
+      <c r="W23" s="1" t="str">
+        <v>Oberta</v>
+      </c>
+      <c r="X23" s="1" t="str">
+        <v>Si, com a primer temps quirúrgic</v>
+      </c>
+      <c r="Y23" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="Z23" s="1" t="str">
+        <v>Impressió R1</v>
+      </c>
+      <c r="AA23" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB23" s="1">
+        <v>3</v>
+      </c>
+      <c r="AC23" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AD23" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AE23" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AF23" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AG23" s="1" t="str">
+        <v>IIIb</v>
+      </c>
+      <c r="AH23" s="1">
+        <v>61</v>
+      </c>
+      <c r="AI23" s="1">
+        <v>1</v>
+      </c>
+      <c r="AJ23" s="1">
+        <v>3</v>
+      </c>
+      <c r="AK23" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL23" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AM23" s="1" t="str">
+        <v>ampliacio quirurgica</v>
+      </c>
+      <c r="AN23" s="2">
+        <v>43983</v>
+      </c>
+      <c r="AO23" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AP23" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AQ23" s="1" t="str">
+        <v>Viu</v>
+      </c>
+      <c r="AR23" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AS23" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AT23" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AU23" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AV23" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AW23" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AX23" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AY23" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AZ23" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BA23" s="1">
+        <v>55</v>
+      </c>
+      <c r="BB23" s="2">
+        <v>44608.380268472225</v>
+      </c>
+      <c r="BC23" s="2">
+        <v>43446</v>
+      </c>
+      <c r="BD23" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BG23" s="1" t="str">
+        <v>oclusió, peritonitis fecaoidea</v>
+      </c>
+      <c r="BH23" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="str">
+        <v>Hepatectomia dreta</v>
+      </c>
+      <c r="B24" s="1">
+        <v>1695</v>
+      </c>
+      <c r="C24" s="1" t="str">
+        <v>09/07/2018</v>
+      </c>
+      <c r="D24" s="1" t="str">
+        <v>11/02/2019</v>
+      </c>
+      <c r="E24" s="1" t="str">
+        <v>25/06/2018</v>
+      </c>
+      <c r="F24" s="1" t="str">
+        <v>VII</v>
+      </c>
+      <c r="H24" s="1" t="str">
+        <v>Jordi</v>
+      </c>
+      <c r="I24" s="1" t="str">
+        <v>Morillas2</v>
+      </c>
+      <c r="J24" s="1" t="str">
+        <v>Esteban2</v>
+      </c>
+      <c r="K24" s="1">
+        <v>13296015</v>
+      </c>
+      <c r="L24" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="O24" s="1" t="str">
+        <v>79</v>
+      </c>
+      <c r="P24" s="1">
+        <v>178</v>
+      </c>
+      <c r="Q24" s="1">
+        <v>25</v>
+      </c>
+      <c r="R24" s="1">
+        <v>3</v>
+      </c>
+      <c r="S24" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="T24" s="2">
+        <v>43858</v>
+      </c>
+      <c r="U24" s="1" t="str">
+        <v>Resecció Major (&gt;= 3 segm)</v>
+      </c>
+      <c r="V24" s="1" t="str">
+        <v>hepatectomia dreta</v>
+      </c>
+      <c r="W24" s="1" t="str">
+        <v>Oberta</v>
+      </c>
+      <c r="X24" s="1" t="str">
+        <v>Si, com a primer temps quirúrgic</v>
+      </c>
+      <c r="Y24" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="Z24" s="1" t="str">
+        <v>Impressió R1</v>
+      </c>
+      <c r="AA24" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB24" s="1">
+        <v>3</v>
+      </c>
+      <c r="AC24" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AD24" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AE24" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AF24" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AG24" s="1" t="str">
+        <v>IIIb</v>
+      </c>
+      <c r="AH24" s="1">
+        <v>61</v>
+      </c>
+      <c r="AI24" s="1">
+        <v>1</v>
+      </c>
+      <c r="AJ24" s="1">
+        <v>3</v>
+      </c>
+      <c r="AK24" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL24" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AM24" s="1" t="str">
+        <v>ampliacio quirurgica</v>
+      </c>
+      <c r="AN24" s="2">
+        <v>43983</v>
+      </c>
+      <c r="AO24" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AP24" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AQ24" s="1" t="str">
+        <v>Viu</v>
+      </c>
+      <c r="AR24" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AS24" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AT24" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AU24" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AV24" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AW24" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AX24" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AY24" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AZ24" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BA24" s="1">
+        <v>55</v>
+      </c>
+      <c r="BB24" s="2">
+        <v>44608.3833528125</v>
+      </c>
+      <c r="BC24" s="2">
+        <v>43446</v>
+      </c>
+      <c r="BD24" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BG24" s="1" t="str">
+        <v>oclusió, peritonitis fecaoidea</v>
+      </c>
+      <c r="BH24" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="str">
+        <v>Hepatectomia dreta</v>
+      </c>
+      <c r="B25" s="1">
+        <v>1695</v>
+      </c>
+      <c r="C25" s="1" t="str">
+        <v>09/07/2018</v>
+      </c>
+      <c r="D25" s="1" t="str">
+        <v>11/02/2019</v>
+      </c>
+      <c r="E25" s="1" t="str">
+        <v>25/06/2018</v>
+      </c>
+      <c r="F25" s="1" t="str">
+        <v>VII</v>
+      </c>
+      <c r="H25" s="1" t="str">
+        <v>Jordi</v>
+      </c>
+      <c r="I25" s="1" t="str">
+        <v>Morillas2</v>
+      </c>
+      <c r="J25" s="1" t="str">
+        <v>Esteban2</v>
+      </c>
+      <c r="K25" s="1">
+        <v>13296015</v>
+      </c>
+      <c r="L25" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="O25" s="1" t="str">
+        <v>79</v>
+      </c>
+      <c r="P25" s="1">
+        <v>178</v>
+      </c>
+      <c r="Q25" s="1">
+        <v>25</v>
+      </c>
+      <c r="R25" s="1">
+        <v>3</v>
+      </c>
+      <c r="S25" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="T25" s="2">
+        <v>43858</v>
+      </c>
+      <c r="U25" s="1" t="str">
+        <v>Resecció Major (&gt;= 3 segm)</v>
+      </c>
+      <c r="V25" s="1" t="str">
+        <v>hepatectomia dreta</v>
+      </c>
+      <c r="W25" s="1" t="str">
+        <v>Oberta</v>
+      </c>
+      <c r="X25" s="1" t="str">
+        <v>Si, com a primer temps quirúrgic</v>
+      </c>
+      <c r="Y25" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="Z25" s="1" t="str">
+        <v>Impressió R1</v>
+      </c>
+      <c r="AA25" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB25" s="1">
+        <v>3</v>
+      </c>
+      <c r="AC25" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AD25" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AE25" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AF25" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AG25" s="1" t="str">
+        <v>IIIb</v>
+      </c>
+      <c r="AH25" s="1">
+        <v>61</v>
+      </c>
+      <c r="AI25" s="1">
+        <v>1</v>
+      </c>
+      <c r="AJ25" s="1">
+        <v>3</v>
+      </c>
+      <c r="AK25" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL25" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AM25" s="1" t="str">
+        <v>ampliacio quirurgica</v>
+      </c>
+      <c r="AN25" s="2">
+        <v>43983</v>
+      </c>
+      <c r="AO25" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AP25" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AQ25" s="1" t="str">
+        <v>Viu</v>
+      </c>
+      <c r="AR25" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AS25" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AT25" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AU25" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AV25" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AW25" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AX25" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AY25" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AZ25" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BA25" s="1">
+        <v>55</v>
+      </c>
+      <c r="BB25" s="2">
+        <v>44608.38351642361</v>
+      </c>
+      <c r="BC25" s="2">
+        <v>43446</v>
+      </c>
+      <c r="BD25" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BG25" s="1" t="str">
+        <v>oclusió, peritonitis fecaoidea</v>
+      </c>
+      <c r="BH25" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="str">
+        <v>Hepatectomia dreta</v>
+      </c>
+      <c r="B26" s="1">
+        <v>1695</v>
+      </c>
+      <c r="C26" s="1" t="str">
+        <v>09/07/2018</v>
+      </c>
+      <c r="D26" s="1" t="str">
+        <v>11/02/2019</v>
+      </c>
+      <c r="E26" s="1" t="str">
+        <v>25/06/2018</v>
+      </c>
+      <c r="F26" s="1" t="str">
+        <v>VII</v>
+      </c>
+      <c r="H26" s="1" t="str">
+        <v>Jordi</v>
+      </c>
+      <c r="I26" s="1" t="str">
+        <v>Morillas2</v>
+      </c>
+      <c r="J26" s="1" t="str">
+        <v>Esteban2</v>
+      </c>
+      <c r="K26" s="1">
+        <v>13296015</v>
+      </c>
+      <c r="L26" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="O26" s="1" t="str">
+        <v>79</v>
+      </c>
+      <c r="P26" s="1">
+        <v>178</v>
+      </c>
+      <c r="Q26" s="1">
+        <v>25</v>
+      </c>
+      <c r="R26" s="1">
+        <v>3</v>
+      </c>
+      <c r="S26" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="T26" s="2">
+        <v>43858</v>
+      </c>
+      <c r="U26" s="1" t="str">
+        <v>Resecció Major (&gt;= 3 segm)</v>
+      </c>
+      <c r="V26" s="1" t="str">
+        <v>hepatectomia dreta</v>
+      </c>
+      <c r="W26" s="1" t="str">
+        <v>Oberta</v>
+      </c>
+      <c r="X26" s="1" t="str">
+        <v>Si, com a primer temps quirúrgic</v>
+      </c>
+      <c r="Y26" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="Z26" s="1" t="str">
+        <v>Impressió R1</v>
+      </c>
+      <c r="AA26" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB26" s="1">
+        <v>3</v>
+      </c>
+      <c r="AC26" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AD26" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AE26" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AF26" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AG26" s="1" t="str">
+        <v>IIIb</v>
+      </c>
+      <c r="AH26" s="1">
+        <v>61</v>
+      </c>
+      <c r="AI26" s="1">
+        <v>1</v>
+      </c>
+      <c r="AJ26" s="1">
+        <v>3</v>
+      </c>
+      <c r="AK26" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL26" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AM26" s="1" t="str">
+        <v>ampliacio quirurgica</v>
+      </c>
+      <c r="AN26" s="2">
+        <v>43983</v>
+      </c>
+      <c r="AO26" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AP26" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AQ26" s="1" t="str">
+        <v>Viu</v>
+      </c>
+      <c r="AR26" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AS26" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AT26" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AU26" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AV26" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AW26" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AX26" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AY26" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AZ26" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BA26" s="1">
+        <v>55</v>
+      </c>
+      <c r="BB26" s="2">
+        <v>44608.38608322917</v>
+      </c>
+      <c r="BC26" s="2">
+        <v>43446</v>
+      </c>
+      <c r="BD26" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BG26" s="1" t="str">
+        <v>oclusió, peritonitis fecaoidea</v>
+      </c>
+      <c r="BH26" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="str">
+        <v>Hepatectomia dreta</v>
+      </c>
+      <c r="B27" s="1">
+        <v>1695</v>
+      </c>
+      <c r="C27" s="1" t="str">
+        <v>09/07/2018</v>
+      </c>
+      <c r="D27" s="1" t="str">
+        <v>11/02/2019</v>
+      </c>
+      <c r="E27" s="1" t="str">
+        <v>25/06/2018</v>
+      </c>
+      <c r="F27" s="1" t="str">
+        <v>VII</v>
+      </c>
+      <c r="H27" s="1" t="str">
+        <v>Jordi</v>
+      </c>
+      <c r="I27" s="1" t="str">
+        <v>Morillas2</v>
+      </c>
+      <c r="J27" s="1" t="str">
+        <v>Esteban2</v>
+      </c>
+      <c r="K27" s="1">
+        <v>13296015</v>
+      </c>
+      <c r="L27" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="O27" s="1" t="str">
+        <v>79</v>
+      </c>
+      <c r="P27" s="1">
+        <v>178</v>
+      </c>
+      <c r="Q27" s="1">
+        <v>25</v>
+      </c>
+      <c r="R27" s="1">
+        <v>3</v>
+      </c>
+      <c r="S27" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="T27" s="2">
+        <v>43858</v>
+      </c>
+      <c r="U27" s="1" t="str">
+        <v>Resecció Major (&gt;= 3 segm)</v>
+      </c>
+      <c r="V27" s="1" t="str">
+        <v>hepatectomia dreta</v>
+      </c>
+      <c r="W27" s="1" t="str">
+        <v>Oberta</v>
+      </c>
+      <c r="X27" s="1" t="str">
+        <v>Si, com a primer temps quirúrgic</v>
+      </c>
+      <c r="Y27" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="Z27" s="1" t="str">
+        <v>Impressió R1</v>
+      </c>
+      <c r="AA27" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB27" s="1">
+        <v>3</v>
+      </c>
+      <c r="AC27" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AD27" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AE27" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AF27" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AG27" s="1" t="str">
+        <v>IIIb</v>
+      </c>
+      <c r="AH27" s="1">
+        <v>61</v>
+      </c>
+      <c r="AI27" s="1">
+        <v>1</v>
+      </c>
+      <c r="AJ27" s="1">
+        <v>3</v>
+      </c>
+      <c r="AK27" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL27" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AM27" s="1" t="str">
+        <v>ampliacio quirurgica</v>
+      </c>
+      <c r="AN27" s="2">
+        <v>43983</v>
+      </c>
+      <c r="AO27" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AP27" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AQ27" s="1" t="str">
+        <v>Viu</v>
+      </c>
+      <c r="AR27" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AS27" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AT27" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AU27" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AV27" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AW27" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AX27" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AY27" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AZ27" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BA27" s="1">
+        <v>55</v>
+      </c>
+      <c r="BB27" s="2">
+        <v>44608.38652545139</v>
+      </c>
+      <c r="BC27" s="2">
+        <v>43446</v>
+      </c>
+      <c r="BD27" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BG27" s="1" t="str">
+        <v>oclusió, peritonitis fecaoidea</v>
+      </c>
+      <c r="BH27" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="str">
+        <v>Hepatectomia dreta</v>
+      </c>
+      <c r="B28" s="1">
+        <v>1695</v>
+      </c>
+      <c r="C28" s="1" t="str">
+        <v>09/07/2018</v>
+      </c>
+      <c r="D28" s="1" t="str">
+        <v>11/02/2019</v>
+      </c>
+      <c r="E28" s="1" t="str">
+        <v>25/06/2018</v>
+      </c>
+      <c r="F28" s="1" t="str">
+        <v>VII</v>
+      </c>
+      <c r="H28" s="1" t="str">
+        <v>Jordi</v>
+      </c>
+      <c r="I28" s="1" t="str">
+        <v>Morillas2</v>
+      </c>
+      <c r="J28" s="1" t="str">
+        <v>Esteban2</v>
+      </c>
+      <c r="K28" s="1">
+        <v>13296015</v>
+      </c>
+      <c r="L28" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="O28" s="1" t="str">
+        <v>79</v>
+      </c>
+      <c r="P28" s="1">
+        <v>178</v>
+      </c>
+      <c r="Q28" s="1">
+        <v>25</v>
+      </c>
+      <c r="R28" s="1">
+        <v>3</v>
+      </c>
+      <c r="S28" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="T28" s="2">
+        <v>43858</v>
+      </c>
+      <c r="U28" s="1" t="str">
+        <v>Resecció Major (&gt;= 3 segm)</v>
+      </c>
+      <c r="V28" s="1" t="str">
+        <v>hepatectomia dreta</v>
+      </c>
+      <c r="W28" s="1" t="str">
+        <v>Oberta</v>
+      </c>
+      <c r="X28" s="1" t="str">
+        <v>Si, com a primer temps quirúrgic</v>
+      </c>
+      <c r="Y28" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="Z28" s="1" t="str">
+        <v>Impressió R1</v>
+      </c>
+      <c r="AA28" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB28" s="1">
+        <v>3</v>
+      </c>
+      <c r="AC28" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AD28" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AE28" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AF28" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AG28" s="1" t="str">
+        <v>IIIb</v>
+      </c>
+      <c r="AH28" s="1">
+        <v>61</v>
+      </c>
+      <c r="AI28" s="1">
+        <v>1</v>
+      </c>
+      <c r="AJ28" s="1">
+        <v>3</v>
+      </c>
+      <c r="AK28" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL28" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AM28" s="1" t="str">
+        <v>ampliacio quirurgica</v>
+      </c>
+      <c r="AN28" s="2">
+        <v>43983</v>
+      </c>
+      <c r="AO28" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AP28" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AQ28" s="1" t="str">
+        <v>Viu</v>
+      </c>
+      <c r="AR28" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AS28" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AT28" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AU28" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AV28" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AW28" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AX28" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AY28" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AZ28" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BA28" s="1">
+        <v>55</v>
+      </c>
+      <c r="BB28" s="2">
+        <v>44608.38744711805</v>
+      </c>
+      <c r="BC28" s="2">
+        <v>43446</v>
+      </c>
+      <c r="BD28" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BG28" s="1" t="str">
+        <v>oclusió, peritonitis fecaoidea</v>
+      </c>
+      <c r="BH28" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="str">
+        <v>Hepatectomia dreta</v>
+      </c>
+      <c r="B29" s="1">
+        <v>1695</v>
+      </c>
+      <c r="C29" s="1" t="str">
+        <v>09/07/2018</v>
+      </c>
+      <c r="D29" s="1" t="str">
+        <v>11/02/2019</v>
+      </c>
+      <c r="E29" s="1" t="str">
+        <v>25/06/2018</v>
+      </c>
+      <c r="F29" s="1" t="str">
+        <v>VII</v>
+      </c>
+      <c r="H29" s="1" t="str">
+        <v>Jordi</v>
+      </c>
+      <c r="I29" s="1" t="str">
+        <v>Morillas2</v>
+      </c>
+      <c r="J29" s="1" t="str">
+        <v>Esteban2</v>
+      </c>
+      <c r="K29" s="1">
+        <v>13296015</v>
+      </c>
+      <c r="L29" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="O29" s="1" t="str">
+        <v>79</v>
+      </c>
+      <c r="P29" s="1">
+        <v>178</v>
+      </c>
+      <c r="Q29" s="1">
+        <v>25</v>
+      </c>
+      <c r="R29" s="1">
+        <v>3</v>
+      </c>
+      <c r="S29" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="T29" s="2">
+        <v>43858</v>
+      </c>
+      <c r="U29" s="1" t="str">
+        <v>Resecció Major (&gt;= 3 segm)</v>
+      </c>
+      <c r="V29" s="1" t="str">
+        <v>hepatectomia dreta</v>
+      </c>
+      <c r="W29" s="1" t="str">
+        <v>Oberta</v>
+      </c>
+      <c r="X29" s="1" t="str">
+        <v>Si, com a primer temps quirúrgic</v>
+      </c>
+      <c r="Y29" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="Z29" s="1" t="str">
+        <v>Impressió R1</v>
+      </c>
+      <c r="AA29" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB29" s="1">
+        <v>3</v>
+      </c>
+      <c r="AC29" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AD29" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AE29" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AF29" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AG29" s="1" t="str">
+        <v>IIIb</v>
+      </c>
+      <c r="AH29" s="1">
+        <v>61</v>
+      </c>
+      <c r="AI29" s="1">
+        <v>1</v>
+      </c>
+      <c r="AJ29" s="1">
+        <v>3</v>
+      </c>
+      <c r="AK29" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL29" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AM29" s="1" t="str">
+        <v>ampliacio quirurgica</v>
+      </c>
+      <c r="AN29" s="2">
+        <v>43983</v>
+      </c>
+      <c r="AO29" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AP29" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AQ29" s="1" t="str">
+        <v>Viu</v>
+      </c>
+      <c r="AR29" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AS29" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AT29" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AU29" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AV29" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AW29" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AX29" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AY29" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AZ29" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BA29" s="1">
+        <v>55</v>
+      </c>
+      <c r="BB29" s="2">
+        <v>44608.38789902778</v>
+      </c>
+      <c r="BC29" s="2">
+        <v>43446</v>
+      </c>
+      <c r="BD29" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BG29" s="1" t="str">
+        <v>oclusió, peritonitis fecaoidea</v>
+      </c>
+      <c r="BH29" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="str">
+        <v>Hepatectomia dreta</v>
+      </c>
+      <c r="B30" s="1">
+        <v>1695</v>
+      </c>
+      <c r="C30" s="1" t="str">
+        <v>09/07/2018</v>
+      </c>
+      <c r="D30" s="1" t="str">
+        <v>11/02/2019</v>
+      </c>
+      <c r="E30" s="1" t="str">
+        <v>25/06/2018</v>
+      </c>
+      <c r="F30" s="1" t="str">
+        <v>VII</v>
+      </c>
+      <c r="H30" s="1" t="str">
+        <v>Jordi</v>
+      </c>
+      <c r="I30" s="1" t="str">
+        <v>Morillas2</v>
+      </c>
+      <c r="J30" s="1" t="str">
+        <v>Esteban2</v>
+      </c>
+      <c r="K30" s="1">
+        <v>13296015</v>
+      </c>
+      <c r="L30" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="O30" s="1" t="str">
+        <v>79</v>
+      </c>
+      <c r="P30" s="1">
+        <v>178</v>
+      </c>
+      <c r="Q30" s="1">
+        <v>25</v>
+      </c>
+      <c r="R30" s="1">
+        <v>3</v>
+      </c>
+      <c r="S30" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="T30" s="2">
+        <v>43858</v>
+      </c>
+      <c r="U30" s="1" t="str">
+        <v>Resecció Major (&gt;= 3 segm)</v>
+      </c>
+      <c r="V30" s="1" t="str">
+        <v>hepatectomia dreta</v>
+      </c>
+      <c r="W30" s="1" t="str">
+        <v>Oberta</v>
+      </c>
+      <c r="X30" s="1" t="str">
+        <v>Si, com a primer temps quirúrgic</v>
+      </c>
+      <c r="Y30" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="Z30" s="1" t="str">
+        <v>Impressió R1</v>
+      </c>
+      <c r="AA30" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB30" s="1">
+        <v>3</v>
+      </c>
+      <c r="AC30" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AD30" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AE30" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AF30" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AG30" s="1" t="str">
+        <v>IIIb</v>
+      </c>
+      <c r="AH30" s="1">
+        <v>61</v>
+      </c>
+      <c r="AI30" s="1">
+        <v>1</v>
+      </c>
+      <c r="AJ30" s="1">
+        <v>3</v>
+      </c>
+      <c r="AK30" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL30" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AM30" s="1" t="str">
+        <v>ampliacio quirurgica</v>
+      </c>
+      <c r="AN30" s="2">
+        <v>43983</v>
+      </c>
+      <c r="AO30" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AP30" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AQ30" s="1" t="str">
+        <v>Viu</v>
+      </c>
+      <c r="AR30" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AS30" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AT30" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AU30" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AV30" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AW30" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AX30" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AY30" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AZ30" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BA30" s="1">
+        <v>55</v>
+      </c>
+      <c r="BB30" s="2">
+        <v>44608.38863931713</v>
+      </c>
+      <c r="BC30" s="2">
+        <v>43446</v>
+      </c>
+      <c r="BD30" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BG30" s="1" t="str">
+        <v>oclusió, peritonitis fecaoidea</v>
+      </c>
+      <c r="BH30" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="str">
+        <v>Hepatectomia dreta</v>
+      </c>
+      <c r="B31" s="1">
+        <v>1695</v>
+      </c>
+      <c r="C31" s="1" t="str">
+        <v>09/07/2018</v>
+      </c>
+      <c r="D31" s="1" t="str">
+        <v>11/02/2019</v>
+      </c>
+      <c r="E31" s="1" t="str">
+        <v>25/06/2018</v>
+      </c>
+      <c r="F31" s="1" t="str">
+        <v>VII</v>
+      </c>
+      <c r="H31" s="1" t="str">
+        <v>Jordi</v>
+      </c>
+      <c r="I31" s="1" t="str">
+        <v>Morillas2</v>
+      </c>
+      <c r="J31" s="1" t="str">
+        <v>Esteban2</v>
+      </c>
+      <c r="K31" s="1">
+        <v>13296015</v>
+      </c>
+      <c r="L31" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="O31" s="1" t="str">
+        <v>79</v>
+      </c>
+      <c r="P31" s="1">
+        <v>178</v>
+      </c>
+      <c r="Q31" s="1">
+        <v>25</v>
+      </c>
+      <c r="R31" s="1">
+        <v>3</v>
+      </c>
+      <c r="S31" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="T31" s="2">
+        <v>43858</v>
+      </c>
+      <c r="U31" s="1" t="str">
+        <v>Resecció Major (&gt;= 3 segm)</v>
+      </c>
+      <c r="V31" s="1" t="str">
+        <v>hepatectomia dreta</v>
+      </c>
+      <c r="W31" s="1" t="str">
+        <v>Oberta</v>
+      </c>
+      <c r="X31" s="1" t="str">
+        <v>Si, com a primer temps quirúrgic</v>
+      </c>
+      <c r="Y31" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="Z31" s="1" t="str">
+        <v>Impressió R1</v>
+      </c>
+      <c r="AA31" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB31" s="1">
+        <v>3</v>
+      </c>
+      <c r="AC31" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AD31" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AE31" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AF31" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AG31" s="1" t="str">
+        <v>IIIb</v>
+      </c>
+      <c r="AH31" s="1">
+        <v>61</v>
+      </c>
+      <c r="AI31" s="1">
+        <v>1</v>
+      </c>
+      <c r="AJ31" s="1">
+        <v>3</v>
+      </c>
+      <c r="AK31" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL31" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AM31" s="1" t="str">
+        <v>ampliacio quirurgica</v>
+      </c>
+      <c r="AN31" s="2">
+        <v>43983</v>
+      </c>
+      <c r="AO31" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AP31" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AQ31" s="1" t="str">
+        <v>Viu</v>
+      </c>
+      <c r="AR31" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AS31" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AT31" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AU31" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AV31" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AW31" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AX31" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AY31" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AZ31" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BA31" s="1">
+        <v>55</v>
+      </c>
+      <c r="BB31" s="2">
+        <v>44608.40377138889</v>
+      </c>
+      <c r="BC31" s="2">
+        <v>43446</v>
+      </c>
+      <c r="BD31" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BG31" s="1" t="str">
+        <v>oclusió, peritonitis fecaoidea</v>
+      </c>
+      <c r="BH31" s="1">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:BF16"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:BH31"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add inputs for brisbane and correct clavien
</commit_message>
<xml_diff>
--- a/register/completedRegister.xlsx
+++ b/register/completedRegister.xlsx
@@ -379,7 +379,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BI37"/>
+  <dimension ref="A1:BJ54"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -568,6 +568,9 @@
       <c r="BI1" s="1" t="str">
         <v>Data EXITUS</v>
       </c>
+      <c r="BJ1" s="1" t="str">
+        <v>BRISBANE</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="str">
@@ -6467,9 +6470,2857 @@
         <v>43708</v>
       </c>
     </row>
+    <row r="38">
+      <c r="A38" s="1" t="str">
+        <v>Resecció/ns limitada/es</v>
+      </c>
+      <c r="B38" s="1">
+        <v>1671</v>
+      </c>
+      <c r="C38" s="1" t="str">
+        <v>05/04/2019</v>
+      </c>
+      <c r="D38" s="1" t="str">
+        <v>05/04/2019</v>
+      </c>
+      <c r="E38" s="1" t="str">
+        <v>28/12/2016</v>
+      </c>
+      <c r="F38" s="1" t="str">
+        <v>VIII</v>
+      </c>
+      <c r="G38" s="1">
+        <v>1415</v>
+      </c>
+      <c r="H38" s="1" t="str">
+        <v>Josep M2</v>
+      </c>
+      <c r="I38" s="1" t="str">
+        <v>Balleste2</v>
+      </c>
+      <c r="J38" s="1" t="str">
+        <v>Blasco2</v>
+      </c>
+      <c r="K38" s="1">
+        <v>10207678</v>
+      </c>
+      <c r="L38" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="M38" s="1" t="str">
+        <v>Home</v>
+      </c>
+      <c r="N38" s="1" t="str">
+        <v>75</v>
+      </c>
+      <c r="O38" s="1" t="str">
+        <v>73</v>
+      </c>
+      <c r="P38" s="1">
+        <v>166</v>
+      </c>
+      <c r="Q38" s="1">
+        <v>27</v>
+      </c>
+      <c r="R38" s="1">
+        <v>3</v>
+      </c>
+      <c r="S38" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="T38" s="2">
+        <v>43686</v>
+      </c>
+      <c r="U38" s="1" t="str">
+        <v>Resecció Menor (&lt;3 segm)</v>
+      </c>
+      <c r="V38" s="1" t="str">
+        <v>dues RL segment8</v>
+      </c>
+      <c r="W38" s="1" t="str">
+        <v>Oberta</v>
+      </c>
+      <c r="X38" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="Y38" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="Z38" s="1" t="str">
+        <v>Impressió R1</v>
+      </c>
+      <c r="AA38" s="1">
+        <v>2</v>
+      </c>
+      <c r="AB38" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD38" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AE38" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AF38" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AG38" s="1" t="str">
+        <v>V</v>
+      </c>
+      <c r="AH38" s="1">
+        <v>100</v>
+      </c>
+      <c r="AN38" s="2">
+        <v>43708</v>
+      </c>
+      <c r="AO38" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AP38" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AQ38" s="1" t="str">
+        <v>Mort (lliure malaltia)</v>
+      </c>
+      <c r="AR38" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AS38" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AT38" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AU38" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AV38" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AW38" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AX38" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BA38" s="1">
+        <v>23</v>
+      </c>
+      <c r="BB38" s="2">
+        <v>44610.43954850695</v>
+      </c>
+      <c r="BC38" s="2">
+        <v>42824</v>
+      </c>
+      <c r="BI38" s="2">
+        <v>43708</v>
+      </c>
+      <c r="BJ38" s="1" t="str">
+        <v>no reglada</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="str">
+        <v>Resecció/ns limitada/es</v>
+      </c>
+      <c r="B39" s="1">
+        <v>1671</v>
+      </c>
+      <c r="C39" s="1" t="str">
+        <v>05/04/2019</v>
+      </c>
+      <c r="D39" s="1" t="str">
+        <v>05/04/2019</v>
+      </c>
+      <c r="E39" s="1" t="str">
+        <v>28/12/2016</v>
+      </c>
+      <c r="F39" s="1" t="str">
+        <v>VIII</v>
+      </c>
+      <c r="G39" s="1">
+        <v>1415</v>
+      </c>
+      <c r="H39" s="1" t="str">
+        <v>Josep M2</v>
+      </c>
+      <c r="I39" s="1" t="str">
+        <v>Balleste2</v>
+      </c>
+      <c r="J39" s="1" t="str">
+        <v>Blasco2</v>
+      </c>
+      <c r="K39" s="1">
+        <v>10207678</v>
+      </c>
+      <c r="L39" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="M39" s="1" t="str">
+        <v>Home</v>
+      </c>
+      <c r="N39" s="1" t="str">
+        <v>75</v>
+      </c>
+      <c r="O39" s="1" t="str">
+        <v>73</v>
+      </c>
+      <c r="P39" s="1">
+        <v>166</v>
+      </c>
+      <c r="Q39" s="1">
+        <v>27</v>
+      </c>
+      <c r="R39" s="1">
+        <v>3</v>
+      </c>
+      <c r="S39" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="T39" s="2">
+        <v>43686</v>
+      </c>
+      <c r="U39" s="1" t="str">
+        <v>Resecció Menor (&lt;3 segm)</v>
+      </c>
+      <c r="V39" s="1" t="str">
+        <v>dues RL segment8</v>
+      </c>
+      <c r="W39" s="1" t="str">
+        <v>Oberta</v>
+      </c>
+      <c r="X39" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="Y39" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="Z39" s="1" t="str">
+        <v>Impressió R1</v>
+      </c>
+      <c r="AA39" s="1">
+        <v>2</v>
+      </c>
+      <c r="AB39" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD39" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AE39" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AF39" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AG39" s="1" t="str">
+        <v>V</v>
+      </c>
+      <c r="AH39" s="1">
+        <v>100</v>
+      </c>
+      <c r="AN39" s="2">
+        <v>43708</v>
+      </c>
+      <c r="AO39" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AP39" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AQ39" s="1" t="str">
+        <v>Mort (lliure malaltia)</v>
+      </c>
+      <c r="AR39" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AS39" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AT39" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AU39" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AV39" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AW39" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AX39" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BA39" s="1">
+        <v>23</v>
+      </c>
+      <c r="BB39" s="2">
+        <v>44610.441321122686</v>
+      </c>
+      <c r="BC39" s="2">
+        <v>42824</v>
+      </c>
+      <c r="BI39" s="2">
+        <v>43708</v>
+      </c>
+      <c r="BJ39" s="1" t="str">
+        <v>no reglada</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="str">
+        <v>Segmentectomia o Bisegmentectomia</v>
+      </c>
+      <c r="B40" s="1">
+        <v>1689</v>
+      </c>
+      <c r="C40" s="1" t="str">
+        <v>03/05/2019</v>
+      </c>
+      <c r="D40" s="1" t="str">
+        <v>20/04/2021</v>
+      </c>
+      <c r="E40" s="1" t="str">
+        <v>13/03/2019</v>
+      </c>
+      <c r="F40" s="1" t="str">
+        <v>VII, VIII</v>
+      </c>
+      <c r="G40" s="1">
+        <v>1545</v>
+      </c>
+      <c r="H40" s="1" t="str">
+        <v>Ana</v>
+      </c>
+      <c r="I40" s="1" t="str">
+        <v>Moral</v>
+      </c>
+      <c r="J40" s="1" t="str">
+        <v>Rueda</v>
+      </c>
+      <c r="K40" s="1">
+        <v>12816340</v>
+      </c>
+      <c r="L40" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="M40" s="1" t="str">
+        <v>Dona</v>
+      </c>
+      <c r="N40" s="1" t="str">
+        <v>69</v>
+      </c>
+      <c r="O40" s="1" t="str">
+        <v>62</v>
+      </c>
+      <c r="P40" s="1">
+        <v>149</v>
+      </c>
+      <c r="Q40" s="1">
+        <v>28</v>
+      </c>
+      <c r="R40" s="1">
+        <v>3</v>
+      </c>
+      <c r="S40" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="T40" s="2">
+        <v>43790</v>
+      </c>
+      <c r="U40" s="1" t="str">
+        <v>Resecció Menor (&lt;3 segm)</v>
+      </c>
+      <c r="V40" s="1" t="str">
+        <v>SEGMENTECTOMIA 4 , rl 6/7 , rl 3  (2)</v>
+      </c>
+      <c r="W40" s="1" t="str">
+        <v>Oberta</v>
+      </c>
+      <c r="X40" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="Y40" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="Z40" s="1" t="str">
+        <v>Impressió R1</v>
+      </c>
+      <c r="AA40" s="1">
+        <v>2</v>
+      </c>
+      <c r="AB40" s="1">
+        <v>2</v>
+      </c>
+      <c r="AC40" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AE40" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AF40" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AG40" s="1" t="str">
+        <v>II</v>
+      </c>
+      <c r="AH40" s="1">
+        <v>29</v>
+      </c>
+      <c r="AI40" s="1">
+        <v>2</v>
+      </c>
+      <c r="AJ40" s="1">
+        <v>2</v>
+      </c>
+      <c r="AK40" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL40" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AM40" s="1" t="str">
+        <v>reseccio. (Ap sense tm)</v>
+      </c>
+      <c r="AN40" s="2">
+        <v>44515</v>
+      </c>
+      <c r="AO40" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AP40" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AQ40" s="1" t="str">
+        <v>Viu</v>
+      </c>
+      <c r="AR40" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AS40" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AT40" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AU40" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AV40" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AW40" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AX40" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AY40" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AZ40" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="BA40" s="1">
+        <v>8</v>
+      </c>
+      <c r="BB40" s="2">
+        <v>44610.441996064816</v>
+      </c>
+      <c r="BC40" s="2">
+        <v>43326</v>
+      </c>
+      <c r="BD40" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BJ40" s="1" t="str">
+        <v>Segmentectomia1a8</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="str">
+        <v>Segmentectomia o Bisegmentectomia</v>
+      </c>
+      <c r="B41" s="1">
+        <v>1689</v>
+      </c>
+      <c r="C41" s="1" t="str">
+        <v>03/05/2019</v>
+      </c>
+      <c r="D41" s="1" t="str">
+        <v>20/04/2021</v>
+      </c>
+      <c r="E41" s="1" t="str">
+        <v>13/03/2019</v>
+      </c>
+      <c r="F41" s="1" t="str">
+        <v>VII, VIII</v>
+      </c>
+      <c r="G41" s="1">
+        <v>1545</v>
+      </c>
+      <c r="H41" s="1" t="str">
+        <v>Ana</v>
+      </c>
+      <c r="I41" s="1" t="str">
+        <v>Moral</v>
+      </c>
+      <c r="J41" s="1" t="str">
+        <v>Rueda</v>
+      </c>
+      <c r="K41" s="1">
+        <v>12816340</v>
+      </c>
+      <c r="L41" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="M41" s="1" t="str">
+        <v>Dona</v>
+      </c>
+      <c r="N41" s="1" t="str">
+        <v>69</v>
+      </c>
+      <c r="O41" s="1" t="str">
+        <v>62</v>
+      </c>
+      <c r="P41" s="1">
+        <v>149</v>
+      </c>
+      <c r="Q41" s="1">
+        <v>28</v>
+      </c>
+      <c r="R41" s="1">
+        <v>3</v>
+      </c>
+      <c r="S41" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="T41" s="2">
+        <v>43790</v>
+      </c>
+      <c r="U41" s="1" t="str">
+        <v>Resecció Menor (&lt;3 segm)</v>
+      </c>
+      <c r="V41" s="1" t="str">
+        <v>SEGMENTECTOMIA 4 , rl 6/7 , rl 3  (2)</v>
+      </c>
+      <c r="W41" s="1" t="str">
+        <v>Oberta</v>
+      </c>
+      <c r="X41" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="Y41" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="Z41" s="1" t="str">
+        <v>Impressió R1</v>
+      </c>
+      <c r="AA41" s="1">
+        <v>2</v>
+      </c>
+      <c r="AB41" s="1">
+        <v>2</v>
+      </c>
+      <c r="AC41" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AE41" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AF41" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AG41" s="1" t="str">
+        <v>II</v>
+      </c>
+      <c r="AH41" s="1">
+        <v>29</v>
+      </c>
+      <c r="AI41" s="1">
+        <v>2</v>
+      </c>
+      <c r="AJ41" s="1">
+        <v>2</v>
+      </c>
+      <c r="AK41" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL41" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AM41" s="1" t="str">
+        <v>reseccio. (Ap sense tm)</v>
+      </c>
+      <c r="AN41" s="2">
+        <v>44515</v>
+      </c>
+      <c r="AO41" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AP41" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AQ41" s="1" t="str">
+        <v>Viu</v>
+      </c>
+      <c r="AR41" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AS41" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AT41" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AU41" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AV41" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AW41" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AX41" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AY41" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AZ41" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="BA41" s="1">
+        <v>8</v>
+      </c>
+      <c r="BB41" s="2">
+        <v>44610.442856932874</v>
+      </c>
+      <c r="BC41" s="2">
+        <v>43326</v>
+      </c>
+      <c r="BD41" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BJ41" s="1" t="str">
+        <v>Segmentectomia1a8</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="str">
+        <v>Segmentectomia o Bisegmentectomia</v>
+      </c>
+      <c r="B42" s="1">
+        <v>1689</v>
+      </c>
+      <c r="C42" s="1" t="str">
+        <v>03/05/2019</v>
+      </c>
+      <c r="D42" s="1" t="str">
+        <v>20/04/2021</v>
+      </c>
+      <c r="E42" s="1" t="str">
+        <v>13/03/2019</v>
+      </c>
+      <c r="F42" s="1" t="str">
+        <v>VII, VIII</v>
+      </c>
+      <c r="G42" s="1">
+        <v>1545</v>
+      </c>
+      <c r="H42" s="1" t="str">
+        <v>Ana</v>
+      </c>
+      <c r="I42" s="1" t="str">
+        <v>Moral</v>
+      </c>
+      <c r="J42" s="1" t="str">
+        <v>Rueda</v>
+      </c>
+      <c r="K42" s="1">
+        <v>12816340</v>
+      </c>
+      <c r="L42" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="M42" s="1" t="str">
+        <v>Dona</v>
+      </c>
+      <c r="N42" s="1" t="str">
+        <v>69</v>
+      </c>
+      <c r="O42" s="1" t="str">
+        <v>62</v>
+      </c>
+      <c r="P42" s="1">
+        <v>149</v>
+      </c>
+      <c r="Q42" s="1">
+        <v>28</v>
+      </c>
+      <c r="R42" s="1">
+        <v>3</v>
+      </c>
+      <c r="S42" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="T42" s="2">
+        <v>43790</v>
+      </c>
+      <c r="U42" s="1" t="str">
+        <v>Resecció Menor (&lt;3 segm)</v>
+      </c>
+      <c r="V42" s="1" t="str">
+        <v>SEGMENTECTOMIA 4 , rl 6/7 , rl 3  (2)</v>
+      </c>
+      <c r="W42" s="1" t="str">
+        <v>Oberta</v>
+      </c>
+      <c r="X42" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="Y42" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="Z42" s="1" t="str">
+        <v>Impressió R1</v>
+      </c>
+      <c r="AA42" s="1">
+        <v>2</v>
+      </c>
+      <c r="AB42" s="1">
+        <v>2</v>
+      </c>
+      <c r="AC42" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AE42" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AF42" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AG42" s="1" t="str">
+        <v>II</v>
+      </c>
+      <c r="AH42" s="1">
+        <v>29</v>
+      </c>
+      <c r="AI42" s="1">
+        <v>2</v>
+      </c>
+      <c r="AJ42" s="1">
+        <v>2</v>
+      </c>
+      <c r="AK42" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL42" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AM42" s="1" t="str">
+        <v>reseccio. (Ap sense tm)</v>
+      </c>
+      <c r="AN42" s="2">
+        <v>44515</v>
+      </c>
+      <c r="AO42" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AP42" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AQ42" s="1" t="str">
+        <v>Viu</v>
+      </c>
+      <c r="AR42" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AS42" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AT42" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AU42" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AV42" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AW42" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AX42" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AY42" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AZ42" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="BA42" s="1">
+        <v>8</v>
+      </c>
+      <c r="BB42" s="2">
+        <v>44610.443434953704</v>
+      </c>
+      <c r="BC42" s="2">
+        <v>43326</v>
+      </c>
+      <c r="BD42" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BJ42" s="1" t="str">
+        <v>Segmentectomia1a8</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="str">
+        <v>Segmentectomia o Bisegmentectomia</v>
+      </c>
+      <c r="B43" s="1">
+        <v>1689</v>
+      </c>
+      <c r="C43" s="1" t="str">
+        <v>03/05/2019</v>
+      </c>
+      <c r="D43" s="1" t="str">
+        <v>20/04/2021</v>
+      </c>
+      <c r="E43" s="1" t="str">
+        <v>13/03/2019</v>
+      </c>
+      <c r="F43" s="1" t="str">
+        <v>VII, VIII</v>
+      </c>
+      <c r="G43" s="1">
+        <v>1545</v>
+      </c>
+      <c r="H43" s="1" t="str">
+        <v>Ana</v>
+      </c>
+      <c r="I43" s="1" t="str">
+        <v>Moral</v>
+      </c>
+      <c r="J43" s="1" t="str">
+        <v>Rueda</v>
+      </c>
+      <c r="K43" s="1">
+        <v>12816340</v>
+      </c>
+      <c r="L43" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="M43" s="1" t="str">
+        <v>Dona</v>
+      </c>
+      <c r="N43" s="1" t="str">
+        <v>69</v>
+      </c>
+      <c r="O43" s="1" t="str">
+        <v>62</v>
+      </c>
+      <c r="P43" s="1">
+        <v>149</v>
+      </c>
+      <c r="Q43" s="1">
+        <v>28</v>
+      </c>
+      <c r="R43" s="1">
+        <v>3</v>
+      </c>
+      <c r="S43" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="T43" s="2">
+        <v>43790</v>
+      </c>
+      <c r="U43" s="1" t="str">
+        <v>Resecció Menor (&lt;3 segm)</v>
+      </c>
+      <c r="V43" s="1" t="str">
+        <v>SEGMENTECTOMIA 4 , rl 6/7 , rl 3  (2)</v>
+      </c>
+      <c r="W43" s="1" t="str">
+        <v>Oberta</v>
+      </c>
+      <c r="X43" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="Y43" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="Z43" s="1" t="str">
+        <v>Impressió R1</v>
+      </c>
+      <c r="AA43" s="1">
+        <v>2</v>
+      </c>
+      <c r="AB43" s="1">
+        <v>2</v>
+      </c>
+      <c r="AC43" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AE43" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AF43" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AG43" s="1" t="str">
+        <v>II</v>
+      </c>
+      <c r="AH43" s="1">
+        <v>29</v>
+      </c>
+      <c r="AI43" s="1">
+        <v>2</v>
+      </c>
+      <c r="AJ43" s="1">
+        <v>2</v>
+      </c>
+      <c r="AK43" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL43" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AM43" s="1" t="str">
+        <v>reseccio. (Ap sense tm)</v>
+      </c>
+      <c r="AN43" s="2">
+        <v>44515</v>
+      </c>
+      <c r="AO43" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AP43" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AQ43" s="1" t="str">
+        <v>Viu</v>
+      </c>
+      <c r="AR43" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AS43" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AT43" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AU43" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AV43" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AW43" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AX43" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AY43" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AZ43" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="BA43" s="1">
+        <v>8</v>
+      </c>
+      <c r="BB43" s="2">
+        <v>44610.44485597222</v>
+      </c>
+      <c r="BC43" s="2">
+        <v>43326</v>
+      </c>
+      <c r="BD43" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BJ43" s="1" t="str">
+        <v>Segmentectomia1a8</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="str">
+        <v>Segmentectomia o Bisegmentectomia</v>
+      </c>
+      <c r="B44" s="1">
+        <v>1689</v>
+      </c>
+      <c r="C44" s="1" t="str">
+        <v>03/05/2019</v>
+      </c>
+      <c r="D44" s="1" t="str">
+        <v>20/04/2021</v>
+      </c>
+      <c r="E44" s="1" t="str">
+        <v>13/03/2019</v>
+      </c>
+      <c r="F44" s="1" t="str">
+        <v>VII, VIII</v>
+      </c>
+      <c r="G44" s="1">
+        <v>1545</v>
+      </c>
+      <c r="H44" s="1" t="str">
+        <v>Ana</v>
+      </c>
+      <c r="I44" s="1" t="str">
+        <v>Moral</v>
+      </c>
+      <c r="J44" s="1" t="str">
+        <v>Rueda</v>
+      </c>
+      <c r="K44" s="1">
+        <v>12816340</v>
+      </c>
+      <c r="L44" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="M44" s="1" t="str">
+        <v>Dona</v>
+      </c>
+      <c r="N44" s="1" t="str">
+        <v>69</v>
+      </c>
+      <c r="O44" s="1" t="str">
+        <v>62</v>
+      </c>
+      <c r="P44" s="1">
+        <v>149</v>
+      </c>
+      <c r="Q44" s="1">
+        <v>28</v>
+      </c>
+      <c r="R44" s="1">
+        <v>3</v>
+      </c>
+      <c r="S44" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="T44" s="2">
+        <v>43790</v>
+      </c>
+      <c r="U44" s="1" t="str">
+        <v>Resecció Menor (&lt;3 segm)</v>
+      </c>
+      <c r="V44" s="1" t="str">
+        <v>SEGMENTECTOMIA 4 , rl 6/7 , rl 3  (2)</v>
+      </c>
+      <c r="W44" s="1" t="str">
+        <v>Oberta</v>
+      </c>
+      <c r="X44" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="Y44" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="Z44" s="1" t="str">
+        <v>Impressió R1</v>
+      </c>
+      <c r="AA44" s="1">
+        <v>2</v>
+      </c>
+      <c r="AB44" s="1">
+        <v>2</v>
+      </c>
+      <c r="AC44" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AE44" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AF44" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AG44" s="1" t="str">
+        <v>II</v>
+      </c>
+      <c r="AH44" s="1">
+        <v>29</v>
+      </c>
+      <c r="AI44" s="1">
+        <v>2</v>
+      </c>
+      <c r="AJ44" s="1">
+        <v>2</v>
+      </c>
+      <c r="AK44" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL44" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AM44" s="1" t="str">
+        <v>reseccio. (Ap sense tm)</v>
+      </c>
+      <c r="AN44" s="2">
+        <v>44515</v>
+      </c>
+      <c r="AO44" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AP44" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AQ44" s="1" t="str">
+        <v>Viu</v>
+      </c>
+      <c r="AR44" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AS44" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AT44" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AU44" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AV44" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AW44" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AX44" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AY44" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AZ44" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="BA44" s="1">
+        <v>8</v>
+      </c>
+      <c r="BB44" s="2">
+        <v>44610.4467818287</v>
+      </c>
+      <c r="BC44" s="2">
+        <v>43326</v>
+      </c>
+      <c r="BD44" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BJ44" s="1" t="str">
+        <v>Segmentectomia1a8</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="str">
+        <v>Segmentectomia o Bisegmentectomia</v>
+      </c>
+      <c r="B45" s="1">
+        <v>1689</v>
+      </c>
+      <c r="C45" s="1" t="str">
+        <v>03/05/2019</v>
+      </c>
+      <c r="D45" s="1" t="str">
+        <v>20/04/2021</v>
+      </c>
+      <c r="E45" s="1" t="str">
+        <v>13/03/2019</v>
+      </c>
+      <c r="F45" s="1" t="str">
+        <v>VII, VIII</v>
+      </c>
+      <c r="G45" s="1">
+        <v>1545</v>
+      </c>
+      <c r="H45" s="1" t="str">
+        <v>Ana</v>
+      </c>
+      <c r="I45" s="1" t="str">
+        <v>Moral</v>
+      </c>
+      <c r="J45" s="1" t="str">
+        <v>Rueda</v>
+      </c>
+      <c r="K45" s="1">
+        <v>12816340</v>
+      </c>
+      <c r="L45" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="M45" s="1" t="str">
+        <v>Dona</v>
+      </c>
+      <c r="N45" s="1" t="str">
+        <v>69</v>
+      </c>
+      <c r="O45" s="1" t="str">
+        <v>62</v>
+      </c>
+      <c r="P45" s="1">
+        <v>149</v>
+      </c>
+      <c r="Q45" s="1">
+        <v>28</v>
+      </c>
+      <c r="R45" s="1">
+        <v>3</v>
+      </c>
+      <c r="S45" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="T45" s="2">
+        <v>43790</v>
+      </c>
+      <c r="U45" s="1" t="str">
+        <v>Resecció Menor (&lt;3 segm)</v>
+      </c>
+      <c r="V45" s="1" t="str">
+        <v>SEGMENTECTOMIA 4 , rl 6/7 , rl 3  (2)</v>
+      </c>
+      <c r="W45" s="1" t="str">
+        <v>Oberta</v>
+      </c>
+      <c r="X45" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="Y45" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="Z45" s="1" t="str">
+        <v>Impressió R1</v>
+      </c>
+      <c r="AA45" s="1">
+        <v>2</v>
+      </c>
+      <c r="AB45" s="1">
+        <v>2</v>
+      </c>
+      <c r="AC45" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AE45" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AF45" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AG45" s="1" t="str">
+        <v>II</v>
+      </c>
+      <c r="AH45" s="1">
+        <v>29</v>
+      </c>
+      <c r="AI45" s="1">
+        <v>2</v>
+      </c>
+      <c r="AJ45" s="1">
+        <v>2</v>
+      </c>
+      <c r="AK45" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL45" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AM45" s="1" t="str">
+        <v>reseccio. (Ap sense tm)</v>
+      </c>
+      <c r="AN45" s="2">
+        <v>44515</v>
+      </c>
+      <c r="AO45" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AP45" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AQ45" s="1" t="str">
+        <v>Viu</v>
+      </c>
+      <c r="AR45" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AS45" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AT45" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AU45" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AV45" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AW45" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AX45" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AY45" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AZ45" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="BA45" s="1">
+        <v>8</v>
+      </c>
+      <c r="BB45" s="2">
+        <v>44610.44750314815</v>
+      </c>
+      <c r="BC45" s="2">
+        <v>43326</v>
+      </c>
+      <c r="BD45" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BJ45" s="1" t="str">
+        <v>Segmentectomia1a8</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="str">
+        <v>Segmentectomia o Bisegmentectomia</v>
+      </c>
+      <c r="B46" s="1">
+        <v>1689</v>
+      </c>
+      <c r="C46" s="1" t="str">
+        <v>03/05/2019</v>
+      </c>
+      <c r="D46" s="1" t="str">
+        <v>20/04/2021</v>
+      </c>
+      <c r="E46" s="1" t="str">
+        <v>13/03/2019</v>
+      </c>
+      <c r="F46" s="1" t="str">
+        <v>VII, VIII</v>
+      </c>
+      <c r="G46" s="1">
+        <v>1545</v>
+      </c>
+      <c r="H46" s="1" t="str">
+        <v>Ana</v>
+      </c>
+      <c r="I46" s="1" t="str">
+        <v>Moral</v>
+      </c>
+      <c r="J46" s="1" t="str">
+        <v>Rueda</v>
+      </c>
+      <c r="K46" s="1">
+        <v>12816340</v>
+      </c>
+      <c r="L46" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="M46" s="1" t="str">
+        <v>Dona</v>
+      </c>
+      <c r="N46" s="1" t="str">
+        <v>69</v>
+      </c>
+      <c r="O46" s="1" t="str">
+        <v>62</v>
+      </c>
+      <c r="P46" s="1">
+        <v>149</v>
+      </c>
+      <c r="Q46" s="1">
+        <v>28</v>
+      </c>
+      <c r="R46" s="1">
+        <v>3</v>
+      </c>
+      <c r="S46" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="T46" s="2">
+        <v>43790</v>
+      </c>
+      <c r="U46" s="1" t="str">
+        <v>Resecció Menor (&lt;3 segm)</v>
+      </c>
+      <c r="V46" s="1" t="str">
+        <v>SEGMENTECTOMIA 4 , rl 6/7 , rl 3  (2)</v>
+      </c>
+      <c r="W46" s="1" t="str">
+        <v>Oberta</v>
+      </c>
+      <c r="X46" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="Y46" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="Z46" s="1" t="str">
+        <v>Impressió R1</v>
+      </c>
+      <c r="AA46" s="1">
+        <v>2</v>
+      </c>
+      <c r="AB46" s="1">
+        <v>2</v>
+      </c>
+      <c r="AC46" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AE46" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AF46" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AG46" s="1" t="str">
+        <v>II</v>
+      </c>
+      <c r="AH46" s="1">
+        <v>29</v>
+      </c>
+      <c r="AI46" s="1">
+        <v>2</v>
+      </c>
+      <c r="AJ46" s="1">
+        <v>2</v>
+      </c>
+      <c r="AK46" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL46" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AM46" s="1" t="str">
+        <v>reseccio. (Ap sense tm)</v>
+      </c>
+      <c r="AN46" s="2">
+        <v>44515</v>
+      </c>
+      <c r="AO46" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AP46" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AQ46" s="1" t="str">
+        <v>Viu</v>
+      </c>
+      <c r="AR46" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AS46" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AT46" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AU46" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AV46" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AW46" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AX46" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AY46" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AZ46" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="BA46" s="1">
+        <v>8</v>
+      </c>
+      <c r="BB46" s="2">
+        <v>44610.44792484953</v>
+      </c>
+      <c r="BC46" s="2">
+        <v>43326</v>
+      </c>
+      <c r="BD46" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BJ46" s="1" t="str">
+        <v>Segmentectomia1a8</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="str">
+        <v>Segmentectomia o Bisegmentectomia</v>
+      </c>
+      <c r="B47" s="1">
+        <v>1689</v>
+      </c>
+      <c r="C47" s="1" t="str">
+        <v>03/05/2019</v>
+      </c>
+      <c r="D47" s="1" t="str">
+        <v>20/04/2021</v>
+      </c>
+      <c r="E47" s="1" t="str">
+        <v>13/03/2019</v>
+      </c>
+      <c r="F47" s="1" t="str">
+        <v>VII, VIII</v>
+      </c>
+      <c r="G47" s="1">
+        <v>1545</v>
+      </c>
+      <c r="H47" s="1" t="str">
+        <v>Ana</v>
+      </c>
+      <c r="I47" s="1" t="str">
+        <v>Moral</v>
+      </c>
+      <c r="J47" s="1" t="str">
+        <v>Rueda</v>
+      </c>
+      <c r="K47" s="1">
+        <v>12816340</v>
+      </c>
+      <c r="L47" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="M47" s="1" t="str">
+        <v>Dona</v>
+      </c>
+      <c r="N47" s="1" t="str">
+        <v>69</v>
+      </c>
+      <c r="O47" s="1" t="str">
+        <v>62</v>
+      </c>
+      <c r="P47" s="1">
+        <v>149</v>
+      </c>
+      <c r="Q47" s="1">
+        <v>28</v>
+      </c>
+      <c r="R47" s="1">
+        <v>3</v>
+      </c>
+      <c r="S47" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="T47" s="2">
+        <v>43790</v>
+      </c>
+      <c r="U47" s="1" t="str">
+        <v>Resecció Menor (&lt;3 segm)</v>
+      </c>
+      <c r="V47" s="1" t="str">
+        <v>SEGMENTECTOMIA 4 , rl 6/7 , rl 3  (2)</v>
+      </c>
+      <c r="W47" s="1" t="str">
+        <v>Oberta</v>
+      </c>
+      <c r="X47" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="Y47" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="Z47" s="1" t="str">
+        <v>Impressió R1</v>
+      </c>
+      <c r="AA47" s="1">
+        <v>2</v>
+      </c>
+      <c r="AB47" s="1">
+        <v>2</v>
+      </c>
+      <c r="AC47" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AE47" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AF47" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AG47" s="1" t="str">
+        <v>II</v>
+      </c>
+      <c r="AH47" s="1">
+        <v>29</v>
+      </c>
+      <c r="AI47" s="1">
+        <v>2</v>
+      </c>
+      <c r="AJ47" s="1">
+        <v>2</v>
+      </c>
+      <c r="AK47" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL47" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AM47" s="1" t="str">
+        <v>reseccio. (Ap sense tm)</v>
+      </c>
+      <c r="AN47" s="2">
+        <v>44515</v>
+      </c>
+      <c r="AO47" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AP47" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AQ47" s="1" t="str">
+        <v>Viu</v>
+      </c>
+      <c r="AR47" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AS47" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AT47" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AU47" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AV47" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AW47" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AX47" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AY47" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AZ47" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="BA47" s="1">
+        <v>8</v>
+      </c>
+      <c r="BB47" s="2">
+        <v>44610.448275497685</v>
+      </c>
+      <c r="BC47" s="2">
+        <v>43326</v>
+      </c>
+      <c r="BD47" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BJ47" s="1" t="str">
+        <v>Segmentectomia1a8</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="str">
+        <v>Segmentectomia o Bisegmentectomia</v>
+      </c>
+      <c r="B48" s="1">
+        <v>1689</v>
+      </c>
+      <c r="C48" s="1" t="str">
+        <v>03/05/2019</v>
+      </c>
+      <c r="D48" s="1" t="str">
+        <v>20/04/2021</v>
+      </c>
+      <c r="E48" s="1" t="str">
+        <v>13/03/2019</v>
+      </c>
+      <c r="F48" s="1" t="str">
+        <v>VII, VIII</v>
+      </c>
+      <c r="G48" s="1">
+        <v>1545</v>
+      </c>
+      <c r="H48" s="1" t="str">
+        <v>Ana</v>
+      </c>
+      <c r="I48" s="1" t="str">
+        <v>Moral</v>
+      </c>
+      <c r="J48" s="1" t="str">
+        <v>Rueda</v>
+      </c>
+      <c r="K48" s="1">
+        <v>12816340</v>
+      </c>
+      <c r="L48" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="M48" s="1" t="str">
+        <v>Dona</v>
+      </c>
+      <c r="N48" s="1" t="str">
+        <v>69</v>
+      </c>
+      <c r="O48" s="1" t="str">
+        <v>62</v>
+      </c>
+      <c r="P48" s="1">
+        <v>149</v>
+      </c>
+      <c r="Q48" s="1">
+        <v>28</v>
+      </c>
+      <c r="R48" s="1">
+        <v>3</v>
+      </c>
+      <c r="S48" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="T48" s="2">
+        <v>43790</v>
+      </c>
+      <c r="U48" s="1" t="str">
+        <v>Resecció Menor (&lt;3 segm)</v>
+      </c>
+      <c r="V48" s="1" t="str">
+        <v>SEGMENTECTOMIA 4 , rl 6/7 , rl 3  (2)</v>
+      </c>
+      <c r="W48" s="1" t="str">
+        <v>Oberta</v>
+      </c>
+      <c r="X48" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="Y48" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="Z48" s="1" t="str">
+        <v>Impressió R1</v>
+      </c>
+      <c r="AA48" s="1">
+        <v>2</v>
+      </c>
+      <c r="AB48" s="1">
+        <v>2</v>
+      </c>
+      <c r="AC48" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AE48" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AF48" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AG48" s="1" t="str">
+        <v>II</v>
+      </c>
+      <c r="AH48" s="1">
+        <v>29</v>
+      </c>
+      <c r="AI48" s="1">
+        <v>2</v>
+      </c>
+      <c r="AJ48" s="1">
+        <v>2</v>
+      </c>
+      <c r="AK48" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL48" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AM48" s="1" t="str">
+        <v>reseccio. (Ap sense tm)</v>
+      </c>
+      <c r="AN48" s="2">
+        <v>44515</v>
+      </c>
+      <c r="AO48" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AP48" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AQ48" s="1" t="str">
+        <v>Viu</v>
+      </c>
+      <c r="AR48" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AS48" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AT48" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AU48" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AV48" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AW48" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AX48" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AY48" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AZ48" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="BA48" s="1">
+        <v>8</v>
+      </c>
+      <c r="BB48" s="2">
+        <v>44610.448518495374</v>
+      </c>
+      <c r="BC48" s="2">
+        <v>43326</v>
+      </c>
+      <c r="BD48" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BJ48" s="1" t="str">
+        <v>Segmentectomia1a8</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="str">
+        <v>Segmentectomia o Bisegmentectomia</v>
+      </c>
+      <c r="B49" s="1">
+        <v>1689</v>
+      </c>
+      <c r="C49" s="1" t="str">
+        <v>03/05/2019</v>
+      </c>
+      <c r="D49" s="1" t="str">
+        <v>20/04/2021</v>
+      </c>
+      <c r="E49" s="1" t="str">
+        <v>13/03/2019</v>
+      </c>
+      <c r="F49" s="1" t="str">
+        <v>VII, VIII</v>
+      </c>
+      <c r="G49" s="1">
+        <v>1545</v>
+      </c>
+      <c r="H49" s="1" t="str">
+        <v>Ana</v>
+      </c>
+      <c r="I49" s="1" t="str">
+        <v>Moral</v>
+      </c>
+      <c r="J49" s="1" t="str">
+        <v>Rueda</v>
+      </c>
+      <c r="K49" s="1">
+        <v>12816340</v>
+      </c>
+      <c r="L49" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="M49" s="1" t="str">
+        <v>Dona</v>
+      </c>
+      <c r="N49" s="1" t="str">
+        <v>69</v>
+      </c>
+      <c r="O49" s="1" t="str">
+        <v>62</v>
+      </c>
+      <c r="P49" s="1">
+        <v>149</v>
+      </c>
+      <c r="Q49" s="1">
+        <v>28</v>
+      </c>
+      <c r="R49" s="1">
+        <v>3</v>
+      </c>
+      <c r="S49" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="T49" s="2">
+        <v>43790</v>
+      </c>
+      <c r="U49" s="1" t="str">
+        <v>Resecció Menor (&lt;3 segm)</v>
+      </c>
+      <c r="V49" s="1" t="str">
+        <v>SEGMENTECTOMIA 4 , rl 6/7 , rl 3  (2)</v>
+      </c>
+      <c r="W49" s="1" t="str">
+        <v>Oberta</v>
+      </c>
+      <c r="X49" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="Y49" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="Z49" s="1" t="str">
+        <v>Impressió R1</v>
+      </c>
+      <c r="AA49" s="1">
+        <v>2</v>
+      </c>
+      <c r="AB49" s="1">
+        <v>2</v>
+      </c>
+      <c r="AC49" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AE49" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AF49" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AG49" s="1" t="str">
+        <v>II</v>
+      </c>
+      <c r="AH49" s="1">
+        <v>29</v>
+      </c>
+      <c r="AI49" s="1">
+        <v>2</v>
+      </c>
+      <c r="AJ49" s="1">
+        <v>2</v>
+      </c>
+      <c r="AK49" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL49" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AM49" s="1" t="str">
+        <v>reseccio. (Ap sense tm)</v>
+      </c>
+      <c r="AN49" s="2">
+        <v>44515</v>
+      </c>
+      <c r="AO49" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AP49" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AQ49" s="1" t="str">
+        <v>Viu</v>
+      </c>
+      <c r="AR49" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AS49" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AT49" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AU49" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AV49" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AW49" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AX49" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AY49" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AZ49" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="BA49" s="1">
+        <v>8</v>
+      </c>
+      <c r="BB49" s="2">
+        <v>44610.462327106485</v>
+      </c>
+      <c r="BC49" s="2">
+        <v>43326</v>
+      </c>
+      <c r="BD49" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BJ49" s="1" t="str">
+        <v>Segmentectomia1a8</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="str">
+        <v>Segmentectomia o Bisegmentectomia</v>
+      </c>
+      <c r="B50" s="1">
+        <v>1689</v>
+      </c>
+      <c r="C50" s="1" t="str">
+        <v>03/05/2019</v>
+      </c>
+      <c r="D50" s="1" t="str">
+        <v>20/04/2021</v>
+      </c>
+      <c r="E50" s="1" t="str">
+        <v>13/03/2019</v>
+      </c>
+      <c r="F50" s="1" t="str">
+        <v>VII, VIII</v>
+      </c>
+      <c r="G50" s="1">
+        <v>1545</v>
+      </c>
+      <c r="H50" s="1" t="str">
+        <v>Ana</v>
+      </c>
+      <c r="I50" s="1" t="str">
+        <v>Moral</v>
+      </c>
+      <c r="J50" s="1" t="str">
+        <v>Rueda</v>
+      </c>
+      <c r="K50" s="1">
+        <v>12816340</v>
+      </c>
+      <c r="L50" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="M50" s="1" t="str">
+        <v>Dona</v>
+      </c>
+      <c r="N50" s="1" t="str">
+        <v>69</v>
+      </c>
+      <c r="O50" s="1" t="str">
+        <v>62</v>
+      </c>
+      <c r="P50" s="1">
+        <v>149</v>
+      </c>
+      <c r="Q50" s="1">
+        <v>28</v>
+      </c>
+      <c r="R50" s="1">
+        <v>3</v>
+      </c>
+      <c r="S50" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="T50" s="2">
+        <v>43790</v>
+      </c>
+      <c r="U50" s="1" t="str">
+        <v>Resecció Menor (&lt;3 segm)</v>
+      </c>
+      <c r="V50" s="1" t="str">
+        <v>SEGMENTECTOMIA 4 , rl 6/7 , rl 3  (2)</v>
+      </c>
+      <c r="W50" s="1" t="str">
+        <v>Oberta</v>
+      </c>
+      <c r="X50" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="Y50" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="Z50" s="1" t="str">
+        <v>Impressió R1</v>
+      </c>
+      <c r="AA50" s="1">
+        <v>2</v>
+      </c>
+      <c r="AB50" s="1">
+        <v>2</v>
+      </c>
+      <c r="AC50" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AE50" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AF50" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AG50" s="1" t="str">
+        <v>II</v>
+      </c>
+      <c r="AH50" s="1">
+        <v>29</v>
+      </c>
+      <c r="AI50" s="1">
+        <v>2</v>
+      </c>
+      <c r="AJ50" s="1">
+        <v>2</v>
+      </c>
+      <c r="AK50" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL50" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AM50" s="1" t="str">
+        <v>reseccio. (Ap sense tm)</v>
+      </c>
+      <c r="AN50" s="2">
+        <v>44515</v>
+      </c>
+      <c r="AO50" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AP50" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AQ50" s="1" t="str">
+        <v>Viu</v>
+      </c>
+      <c r="AR50" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AS50" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AT50" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AU50" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AV50" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AW50" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AX50" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AY50" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AZ50" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="BA50" s="1">
+        <v>8</v>
+      </c>
+      <c r="BB50" s="2">
+        <v>44610.4632481713</v>
+      </c>
+      <c r="BC50" s="2">
+        <v>43326</v>
+      </c>
+      <c r="BD50" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BJ50" s="1" t="str">
+        <v>Segmentectomia1a8</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="str">
+        <v>Segmentectomia o Bisegmentectomia</v>
+      </c>
+      <c r="B51" s="1">
+        <v>1689</v>
+      </c>
+      <c r="C51" s="1" t="str">
+        <v>03/05/2019</v>
+      </c>
+      <c r="D51" s="1" t="str">
+        <v>20/04/2021</v>
+      </c>
+      <c r="E51" s="1" t="str">
+        <v>13/03/2019</v>
+      </c>
+      <c r="F51" s="1" t="str">
+        <v>VII, VIII</v>
+      </c>
+      <c r="G51" s="1">
+        <v>1545</v>
+      </c>
+      <c r="H51" s="1" t="str">
+        <v>Ana</v>
+      </c>
+      <c r="I51" s="1" t="str">
+        <v>Moral</v>
+      </c>
+      <c r="J51" s="1" t="str">
+        <v>Rueda</v>
+      </c>
+      <c r="K51" s="1">
+        <v>12816340</v>
+      </c>
+      <c r="L51" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="M51" s="1" t="str">
+        <v>Dona</v>
+      </c>
+      <c r="N51" s="1" t="str">
+        <v>69</v>
+      </c>
+      <c r="O51" s="1" t="str">
+        <v>62</v>
+      </c>
+      <c r="P51" s="1">
+        <v>149</v>
+      </c>
+      <c r="Q51" s="1">
+        <v>28</v>
+      </c>
+      <c r="R51" s="1">
+        <v>3</v>
+      </c>
+      <c r="S51" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="T51" s="2">
+        <v>43790</v>
+      </c>
+      <c r="U51" s="1" t="str">
+        <v>Resecció Menor (&lt;3 segm)</v>
+      </c>
+      <c r="V51" s="1" t="str">
+        <v>SEGMENTECTOMIA 4 , rl 6/7 , rl 3  (2)</v>
+      </c>
+      <c r="W51" s="1" t="str">
+        <v>Oberta</v>
+      </c>
+      <c r="X51" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="Y51" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="Z51" s="1" t="str">
+        <v>Impressió R1</v>
+      </c>
+      <c r="AA51" s="1">
+        <v>2</v>
+      </c>
+      <c r="AB51" s="1">
+        <v>2</v>
+      </c>
+      <c r="AC51" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AE51" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AF51" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AG51" s="1" t="str">
+        <v>II</v>
+      </c>
+      <c r="AH51" s="1">
+        <v>29</v>
+      </c>
+      <c r="AI51" s="1">
+        <v>2</v>
+      </c>
+      <c r="AJ51" s="1">
+        <v>2</v>
+      </c>
+      <c r="AK51" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL51" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AM51" s="1" t="str">
+        <v>reseccio. (Ap sense tm)</v>
+      </c>
+      <c r="AN51" s="2">
+        <v>44515</v>
+      </c>
+      <c r="AO51" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AP51" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AQ51" s="1" t="str">
+        <v>Viu</v>
+      </c>
+      <c r="AR51" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AS51" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AT51" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AU51" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AV51" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AW51" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AX51" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AY51" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AZ51" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="BA51" s="1">
+        <v>8</v>
+      </c>
+      <c r="BB51" s="2">
+        <v>44610.46345649305</v>
+      </c>
+      <c r="BC51" s="2">
+        <v>43326</v>
+      </c>
+      <c r="BD51" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BJ51" s="1" t="str">
+        <v>Segmentectomia1a8</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="str">
+        <v>Segmentectomia o Bisegmentectomia</v>
+      </c>
+      <c r="B52" s="1">
+        <v>1689</v>
+      </c>
+      <c r="C52" s="1" t="str">
+        <v>03/05/2019</v>
+      </c>
+      <c r="D52" s="1" t="str">
+        <v>20/04/2021</v>
+      </c>
+      <c r="E52" s="1" t="str">
+        <v>13/03/2019</v>
+      </c>
+      <c r="F52" s="1" t="str">
+        <v>VII, VIII</v>
+      </c>
+      <c r="G52" s="1">
+        <v>1545</v>
+      </c>
+      <c r="H52" s="1" t="str">
+        <v>Ana</v>
+      </c>
+      <c r="I52" s="1" t="str">
+        <v>Moral</v>
+      </c>
+      <c r="J52" s="1" t="str">
+        <v>Rueda</v>
+      </c>
+      <c r="K52" s="1">
+        <v>12816340</v>
+      </c>
+      <c r="L52" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="M52" s="1" t="str">
+        <v>Dona</v>
+      </c>
+      <c r="N52" s="1" t="str">
+        <v>69</v>
+      </c>
+      <c r="O52" s="1" t="str">
+        <v>62</v>
+      </c>
+      <c r="P52" s="1">
+        <v>149</v>
+      </c>
+      <c r="Q52" s="1">
+        <v>28</v>
+      </c>
+      <c r="R52" s="1">
+        <v>3</v>
+      </c>
+      <c r="S52" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="T52" s="2">
+        <v>43790</v>
+      </c>
+      <c r="U52" s="1" t="str">
+        <v>Resecció Menor (&lt;3 segm)</v>
+      </c>
+      <c r="V52" s="1" t="str">
+        <v>SEGMENTECTOMIA 4 , rl 6/7 , rl 3  (2)</v>
+      </c>
+      <c r="W52" s="1" t="str">
+        <v>Oberta</v>
+      </c>
+      <c r="X52" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="Y52" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="Z52" s="1" t="str">
+        <v>Impressió R1</v>
+      </c>
+      <c r="AA52" s="1">
+        <v>2</v>
+      </c>
+      <c r="AB52" s="1">
+        <v>2</v>
+      </c>
+      <c r="AC52" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AE52" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AF52" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AG52" s="1" t="str">
+        <v>II</v>
+      </c>
+      <c r="AH52" s="1">
+        <v>29</v>
+      </c>
+      <c r="AI52" s="1">
+        <v>2</v>
+      </c>
+      <c r="AJ52" s="1">
+        <v>2</v>
+      </c>
+      <c r="AK52" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL52" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AM52" s="1" t="str">
+        <v>reseccio. (Ap sense tm)</v>
+      </c>
+      <c r="AN52" s="2">
+        <v>44515</v>
+      </c>
+      <c r="AO52" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AP52" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AQ52" s="1" t="str">
+        <v>Viu</v>
+      </c>
+      <c r="AR52" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AS52" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AT52" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AU52" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AV52" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AW52" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AX52" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AY52" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AZ52" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="BA52" s="1">
+        <v>8</v>
+      </c>
+      <c r="BB52" s="2">
+        <v>44610.46412315972</v>
+      </c>
+      <c r="BC52" s="2">
+        <v>43326</v>
+      </c>
+      <c r="BD52" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BJ52" s="1" t="str">
+        <v>Segmentectomia1a8</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="str">
+        <v>Segmentectomia o Bisegmentectomia</v>
+      </c>
+      <c r="B53" s="1">
+        <v>1689</v>
+      </c>
+      <c r="C53" s="1" t="str">
+        <v>03/05/2019</v>
+      </c>
+      <c r="D53" s="1" t="str">
+        <v>20/04/2021</v>
+      </c>
+      <c r="E53" s="1" t="str">
+        <v>13/03/2019</v>
+      </c>
+      <c r="F53" s="1" t="str">
+        <v>VII, VIII</v>
+      </c>
+      <c r="G53" s="1">
+        <v>1545</v>
+      </c>
+      <c r="H53" s="1" t="str">
+        <v>Ana</v>
+      </c>
+      <c r="I53" s="1" t="str">
+        <v>Moral</v>
+      </c>
+      <c r="J53" s="1" t="str">
+        <v>Rueda</v>
+      </c>
+      <c r="K53" s="1">
+        <v>12816340</v>
+      </c>
+      <c r="L53" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="M53" s="1" t="str">
+        <v>Dona</v>
+      </c>
+      <c r="N53" s="1" t="str">
+        <v>69</v>
+      </c>
+      <c r="O53" s="1" t="str">
+        <v>62</v>
+      </c>
+      <c r="P53" s="1">
+        <v>149</v>
+      </c>
+      <c r="Q53" s="1">
+        <v>28</v>
+      </c>
+      <c r="R53" s="1">
+        <v>3</v>
+      </c>
+      <c r="S53" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="T53" s="2">
+        <v>43790</v>
+      </c>
+      <c r="U53" s="1" t="str">
+        <v>Resecció Menor (&lt;3 segm)</v>
+      </c>
+      <c r="V53" s="1" t="str">
+        <v>SEGMENTECTOMIA 4 , rl 6/7 , rl 3  (2)</v>
+      </c>
+      <c r="W53" s="1" t="str">
+        <v>Oberta</v>
+      </c>
+      <c r="X53" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="Y53" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="Z53" s="1" t="str">
+        <v>Impressió R1</v>
+      </c>
+      <c r="AA53" s="1">
+        <v>2</v>
+      </c>
+      <c r="AB53" s="1">
+        <v>2</v>
+      </c>
+      <c r="AC53" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AE53" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AF53" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AG53" s="1" t="str">
+        <v>II</v>
+      </c>
+      <c r="AH53" s="1">
+        <v>29</v>
+      </c>
+      <c r="AI53" s="1">
+        <v>2</v>
+      </c>
+      <c r="AJ53" s="1">
+        <v>2</v>
+      </c>
+      <c r="AK53" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL53" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AM53" s="1" t="str">
+        <v>reseccio. (Ap sense tm)</v>
+      </c>
+      <c r="AN53" s="2">
+        <v>44515</v>
+      </c>
+      <c r="AO53" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AP53" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AQ53" s="1" t="str">
+        <v>Viu</v>
+      </c>
+      <c r="AR53" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AS53" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AT53" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AU53" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AV53" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AW53" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AX53" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AY53" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AZ53" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="BA53" s="1">
+        <v>8</v>
+      </c>
+      <c r="BB53" s="2">
+        <v>44610.46474826389</v>
+      </c>
+      <c r="BC53" s="2">
+        <v>43326</v>
+      </c>
+      <c r="BD53" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BJ53" s="1" t="str">
+        <v>Segmentectomia1a8</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="str">
+        <v>Segmentectomia o Bisegmentectomia</v>
+      </c>
+      <c r="B54" s="1">
+        <v>1689</v>
+      </c>
+      <c r="C54" s="1" t="str">
+        <v>03/05/2019</v>
+      </c>
+      <c r="D54" s="1" t="str">
+        <v>20/04/2021</v>
+      </c>
+      <c r="E54" s="1" t="str">
+        <v>13/03/2019</v>
+      </c>
+      <c r="F54" s="1" t="str">
+        <v>VII, VIII</v>
+      </c>
+      <c r="G54" s="1">
+        <v>1545</v>
+      </c>
+      <c r="H54" s="1" t="str">
+        <v>Ana</v>
+      </c>
+      <c r="I54" s="1" t="str">
+        <v>Moral</v>
+      </c>
+      <c r="J54" s="1" t="str">
+        <v>Rueda</v>
+      </c>
+      <c r="K54" s="1">
+        <v>12816340</v>
+      </c>
+      <c r="L54" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="M54" s="1" t="str">
+        <v>Dona</v>
+      </c>
+      <c r="N54" s="1" t="str">
+        <v>69</v>
+      </c>
+      <c r="O54" s="1" t="str">
+        <v>62</v>
+      </c>
+      <c r="P54" s="1">
+        <v>149</v>
+      </c>
+      <c r="Q54" s="1">
+        <v>28</v>
+      </c>
+      <c r="R54" s="1">
+        <v>3</v>
+      </c>
+      <c r="S54" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="T54" s="2">
+        <v>43790</v>
+      </c>
+      <c r="U54" s="1" t="str">
+        <v>Resecció Menor (&lt;3 segm)</v>
+      </c>
+      <c r="V54" s="1" t="str">
+        <v>SEGMENTECTOMIA 4 , rl 6/7 , rl 3  (2)</v>
+      </c>
+      <c r="W54" s="1" t="str">
+        <v>Oberta</v>
+      </c>
+      <c r="X54" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="Y54" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="Z54" s="1" t="str">
+        <v>Impressió R1</v>
+      </c>
+      <c r="AA54" s="1">
+        <v>2</v>
+      </c>
+      <c r="AB54" s="1">
+        <v>2</v>
+      </c>
+      <c r="AC54" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AE54" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AF54" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AG54" s="1" t="str">
+        <v>II</v>
+      </c>
+      <c r="AH54" s="1">
+        <v>29</v>
+      </c>
+      <c r="AI54" s="1">
+        <v>2</v>
+      </c>
+      <c r="AJ54" s="1">
+        <v>2</v>
+      </c>
+      <c r="AK54" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL54" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AM54" s="1" t="str">
+        <v>reseccio. (Ap sense tm)</v>
+      </c>
+      <c r="AN54" s="2">
+        <v>44515</v>
+      </c>
+      <c r="AO54" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AP54" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AQ54" s="1" t="str">
+        <v>Viu</v>
+      </c>
+      <c r="AR54" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AS54" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AT54" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AU54" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AV54" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AW54" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AX54" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AY54" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AZ54" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="BA54" s="1">
+        <v>8</v>
+      </c>
+      <c r="BB54" s="2">
+        <v>44610.472465416664</v>
+      </c>
+      <c r="BC54" s="2">
+        <v>43326</v>
+      </c>
+      <c r="BD54" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BJ54" s="1" t="str">
+        <v>Segmentectomia1a8</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:BI37"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:BJ54"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add default values for diagnostics
</commit_message>
<xml_diff>
--- a/register/completedRegister.xlsx
+++ b/register/completedRegister.xlsx
@@ -379,7 +379,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BJ54"/>
+  <dimension ref="A1:BK63"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -571,6 +571,9 @@
       <c r="BJ1" s="1" t="str">
         <v>BRISBANE</v>
       </c>
+      <c r="BK1" s="1" t="str">
+        <v>Grau IH</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="str">
@@ -9318,9 +9321,1500 @@
         <v>Segmentectomia1a8</v>
       </c>
     </row>
+    <row r="55">
+      <c r="A55" s="1" t="str">
+        <v>Segmentectomia o Bisegmentectomia</v>
+      </c>
+      <c r="B55" s="1">
+        <v>1641</v>
+      </c>
+      <c r="C55" s="1" t="str">
+        <v>04/03/2019</v>
+      </c>
+      <c r="D55" s="1" t="str">
+        <v>20/05/2019</v>
+      </c>
+      <c r="E55" s="1" t="str">
+        <v>11/01/2019</v>
+      </c>
+      <c r="F55" s="1" t="str">
+        <v>V</v>
+      </c>
+      <c r="G55" s="1">
+        <v>1504</v>
+      </c>
+      <c r="H55" s="1" t="str">
+        <v>dictino</v>
+      </c>
+      <c r="I55" s="1" t="str">
+        <v>FERNANDEZ</v>
+      </c>
+      <c r="J55" s="1" t="str">
+        <v>ALVAREZ</v>
+      </c>
+      <c r="K55" s="1">
+        <v>13067884</v>
+      </c>
+      <c r="L55" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="M55" s="1" t="str">
+        <v>Home</v>
+      </c>
+      <c r="N55" s="1" t="str">
+        <v>66</v>
+      </c>
+      <c r="O55" s="1" t="str">
+        <v>62</v>
+      </c>
+      <c r="P55" s="1">
+        <v>169</v>
+      </c>
+      <c r="Q55" s="1">
+        <v>22</v>
+      </c>
+      <c r="R55" s="1">
+        <v>2</v>
+      </c>
+      <c r="S55" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="T55" s="2">
+        <v>43546</v>
+      </c>
+      <c r="U55" s="1" t="str">
+        <v>Resecció Menor (&lt;3 segm)</v>
+      </c>
+      <c r="V55" s="1" t="str">
+        <v>segmentectomia 5</v>
+      </c>
+      <c r="W55" s="1" t="str">
+        <v>Oberta</v>
+      </c>
+      <c r="X55" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="Y55" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="Z55" s="1" t="str">
+        <v>Impressió R1</v>
+      </c>
+      <c r="AA55" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB55" s="1">
+        <v>3</v>
+      </c>
+      <c r="AC55" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AD55" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AE55" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AF55" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AG55" s="1" t="str">
+        <v>II</v>
+      </c>
+      <c r="AH55" s="1">
+        <v>21</v>
+      </c>
+      <c r="AI55" s="1">
+        <v>1</v>
+      </c>
+      <c r="AJ55" s="1">
+        <v>2.3</v>
+      </c>
+      <c r="AK55" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL55" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AM55" s="1" t="str">
+        <v>Aquamantis</v>
+      </c>
+      <c r="AN55" s="2">
+        <v>44376</v>
+      </c>
+      <c r="AO55" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AP55" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AQ55" s="1" t="str">
+        <v>Viu</v>
+      </c>
+      <c r="AR55" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AS55" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AT55" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AU55" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AV55" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AW55" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AX55" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AY55" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AZ55" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BA55" s="1">
+        <v>0</v>
+      </c>
+      <c r="BB55" s="2">
+        <v>44610.47735954861</v>
+      </c>
+      <c r="BC55" s="2">
+        <v>43594</v>
+      </c>
+      <c r="BD55" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BJ55" s="1" t="str">
+        <v>Segmentectomia1a8</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="str">
+        <v>Segmentectomia o Bisegmentectomia</v>
+      </c>
+      <c r="B56" s="1">
+        <v>1641</v>
+      </c>
+      <c r="C56" s="1" t="str">
+        <v>04/03/2019</v>
+      </c>
+      <c r="D56" s="1" t="str">
+        <v>20/05/2019</v>
+      </c>
+      <c r="E56" s="1" t="str">
+        <v>11/01/2019</v>
+      </c>
+      <c r="F56" s="1" t="str">
+        <v>V</v>
+      </c>
+      <c r="G56" s="1">
+        <v>1504</v>
+      </c>
+      <c r="H56" s="1" t="str">
+        <v>dictino</v>
+      </c>
+      <c r="I56" s="1" t="str">
+        <v>FERNANDEZ</v>
+      </c>
+      <c r="J56" s="1" t="str">
+        <v>ALVAREZ</v>
+      </c>
+      <c r="K56" s="1">
+        <v>13067884</v>
+      </c>
+      <c r="L56" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="M56" s="1" t="str">
+        <v>Home</v>
+      </c>
+      <c r="N56" s="1" t="str">
+        <v>66</v>
+      </c>
+      <c r="O56" s="1" t="str">
+        <v>62</v>
+      </c>
+      <c r="P56" s="1">
+        <v>169</v>
+      </c>
+      <c r="Q56" s="1">
+        <v>22</v>
+      </c>
+      <c r="R56" s="1">
+        <v>2</v>
+      </c>
+      <c r="S56" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="T56" s="2">
+        <v>43546</v>
+      </c>
+      <c r="U56" s="1" t="str">
+        <v>Resecció Menor (&lt;3 segm)</v>
+      </c>
+      <c r="V56" s="1" t="str">
+        <v>segmentectomia 5</v>
+      </c>
+      <c r="W56" s="1" t="str">
+        <v>Oberta</v>
+      </c>
+      <c r="X56" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="Y56" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="Z56" s="1" t="str">
+        <v>Impressió R1</v>
+      </c>
+      <c r="AA56" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB56" s="1">
+        <v>3</v>
+      </c>
+      <c r="AC56" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AD56" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AE56" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AF56" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AG56" s="1" t="str">
+        <v>II</v>
+      </c>
+      <c r="AH56" s="1">
+        <v>21</v>
+      </c>
+      <c r="AI56" s="1">
+        <v>1</v>
+      </c>
+      <c r="AJ56" s="1">
+        <v>2.3</v>
+      </c>
+      <c r="AK56" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL56" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AM56" s="1" t="str">
+        <v>Aquamantis</v>
+      </c>
+      <c r="AN56" s="2">
+        <v>44376</v>
+      </c>
+      <c r="AO56" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AP56" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AQ56" s="1" t="str">
+        <v>Viu</v>
+      </c>
+      <c r="AR56" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AS56" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AT56" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AU56" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AV56" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AW56" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AX56" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AY56" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AZ56" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BA56" s="1">
+        <v>0</v>
+      </c>
+      <c r="BB56" s="2">
+        <v>44610.47829358796</v>
+      </c>
+      <c r="BC56" s="2">
+        <v>43594</v>
+      </c>
+      <c r="BD56" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BJ56" s="1" t="str">
+        <v>Segmentectomia1a8</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="str">
+        <v>Resecció/ns limitada/es</v>
+      </c>
+      <c r="B57" s="1">
+        <v>1669</v>
+      </c>
+      <c r="C57" s="1" t="str">
+        <v>05/02/2021</v>
+      </c>
+      <c r="D57" s="1" t="str">
+        <v xml:space="preserve">05/02/2021 </v>
+      </c>
+      <c r="E57" s="1" t="str">
+        <v>29/01/2019</v>
+      </c>
+      <c r="F57" s="1" t="str">
+        <v>II,IV,VII,VI,VIII</v>
+      </c>
+      <c r="G57" s="1">
+        <v>1529</v>
+      </c>
+      <c r="H57" s="1" t="str">
+        <v>Salvador</v>
+      </c>
+      <c r="I57" s="1" t="str">
+        <v>Monte</v>
+      </c>
+      <c r="J57" s="1" t="str">
+        <v>Peiro</v>
+      </c>
+      <c r="K57" s="1">
+        <v>13005406</v>
+      </c>
+      <c r="L57" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="M57" s="1" t="str">
+        <v>Home</v>
+      </c>
+      <c r="N57" s="1" t="str">
+        <v>60</v>
+      </c>
+      <c r="O57" s="1">
+        <v>86</v>
+      </c>
+      <c r="P57" s="1">
+        <v>178</v>
+      </c>
+      <c r="R57" s="1">
+        <v>2</v>
+      </c>
+      <c r="T57" s="2">
+        <v>43679</v>
+      </c>
+      <c r="U57" s="1" t="str">
+        <v>Resecció Menor (&lt;3 segm)</v>
+      </c>
+      <c r="V57" s="1" t="str">
+        <v>bisegm 2/3 i 4 RL r0 una d'elles</v>
+      </c>
+      <c r="W57" s="1" t="str">
+        <v>Oberta</v>
+      </c>
+      <c r="X57" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="Y57" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="Z57" s="1" t="str">
+        <v>Impressió R1</v>
+      </c>
+      <c r="AA57" s="1">
+        <v>6</v>
+      </c>
+      <c r="AB57" s="1">
+        <v>2.1</v>
+      </c>
+      <c r="AC57" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AD57" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AE57" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AI57" s="1">
+        <v>7</v>
+      </c>
+      <c r="AJ57" s="1">
+        <v>2.8</v>
+      </c>
+      <c r="AK57" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL57" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AM57" s="1" t="str">
+        <v>aquamantis</v>
+      </c>
+      <c r="AN57" s="2">
+        <v>44525</v>
+      </c>
+      <c r="AO57" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AQ57" s="1" t="str">
+        <v>Viu</v>
+      </c>
+      <c r="AX57" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AY57" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AZ57" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="BB57" s="2">
+        <v>44610.478461516206</v>
+      </c>
+      <c r="BC57" s="2">
+        <v>43525</v>
+      </c>
+      <c r="BD57" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BJ57" s="1" t="str">
+        <v>no reglada</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="str">
+        <v>Hepatectomia dreta</v>
+      </c>
+      <c r="B58" s="1">
+        <v>1695</v>
+      </c>
+      <c r="C58" s="1" t="str">
+        <v>09/07/2018</v>
+      </c>
+      <c r="D58" s="1" t="str">
+        <v>11/02/2019</v>
+      </c>
+      <c r="E58" s="1" t="str">
+        <v>25/06/2018</v>
+      </c>
+      <c r="F58" s="1" t="str">
+        <v>VII</v>
+      </c>
+      <c r="H58" s="1" t="str">
+        <v>Jordi</v>
+      </c>
+      <c r="I58" s="1" t="str">
+        <v>Morillas2</v>
+      </c>
+      <c r="J58" s="1" t="str">
+        <v>Esteban2</v>
+      </c>
+      <c r="K58" s="1">
+        <v>13296015</v>
+      </c>
+      <c r="L58" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="O58" s="1" t="str">
+        <v>79</v>
+      </c>
+      <c r="P58" s="1">
+        <v>178</v>
+      </c>
+      <c r="Q58" s="1">
+        <v>25</v>
+      </c>
+      <c r="R58" s="1">
+        <v>3</v>
+      </c>
+      <c r="S58" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="T58" s="2">
+        <v>43858</v>
+      </c>
+      <c r="U58" s="1" t="str">
+        <v>Resecció Major (&gt;= 3 segm)</v>
+      </c>
+      <c r="V58" s="1" t="str">
+        <v>hepatectomia dreta</v>
+      </c>
+      <c r="W58" s="1" t="str">
+        <v>Oberta</v>
+      </c>
+      <c r="X58" s="1" t="str">
+        <v>Si, com a primer temps quirúrgic</v>
+      </c>
+      <c r="Y58" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="Z58" s="1" t="str">
+        <v>Impressió R1</v>
+      </c>
+      <c r="AA58" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB58" s="1">
+        <v>3</v>
+      </c>
+      <c r="AC58" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AD58" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AE58" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AF58" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AG58" s="1" t="str">
+        <v>IIIb</v>
+      </c>
+      <c r="AH58" s="1">
+        <v>61</v>
+      </c>
+      <c r="AI58" s="1">
+        <v>1</v>
+      </c>
+      <c r="AJ58" s="1">
+        <v>3</v>
+      </c>
+      <c r="AK58" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL58" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AM58" s="1" t="str">
+        <v>ampliacio quirurgica</v>
+      </c>
+      <c r="AN58" s="2">
+        <v>43983</v>
+      </c>
+      <c r="AO58" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AP58" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AQ58" s="1" t="str">
+        <v>Viu</v>
+      </c>
+      <c r="AR58" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AS58" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AT58" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AU58" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AV58" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AW58" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AX58" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AY58" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AZ58" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BA58" s="1">
+        <v>55</v>
+      </c>
+      <c r="BB58" s="2">
+        <v>44610.47960412037</v>
+      </c>
+      <c r="BC58" s="2">
+        <v>43446</v>
+      </c>
+      <c r="BD58" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BG58" s="1" t="str">
+        <v>oclusió, peritonitis fecaoidea</v>
+      </c>
+      <c r="BH58" s="1">
+        <v>2</v>
+      </c>
+      <c r="BJ58" s="1" t="str">
+        <v>hepatectomiaDreta</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="str">
+        <v>Hepatectomia major + resecció contralateral</v>
+      </c>
+      <c r="B59" s="1">
+        <v>1632</v>
+      </c>
+      <c r="C59" s="1" t="str">
+        <v>05/04/2018</v>
+      </c>
+      <c r="D59" s="1" t="str">
+        <v>09/06/2021</v>
+      </c>
+      <c r="E59" s="1" t="str">
+        <v>01/01/2018</v>
+      </c>
+      <c r="F59" s="1" t="str">
+        <v>IV</v>
+      </c>
+      <c r="G59" s="1">
+        <v>1497</v>
+      </c>
+      <c r="H59" s="1" t="str">
+        <v>JAUME</v>
+      </c>
+      <c r="I59" s="1" t="str">
+        <v>GUAL</v>
+      </c>
+      <c r="J59" s="1" t="str">
+        <v>BOSCH</v>
+      </c>
+      <c r="K59" s="1">
+        <v>13297134</v>
+      </c>
+      <c r="L59" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="M59" s="1" t="str">
+        <v>Home</v>
+      </c>
+      <c r="N59" s="1" t="str">
+        <v>47</v>
+      </c>
+      <c r="O59" s="1" t="str">
+        <v>87</v>
+      </c>
+      <c r="P59" s="1">
+        <v>170</v>
+      </c>
+      <c r="Q59" s="1">
+        <v>30</v>
+      </c>
+      <c r="R59" s="1">
+        <v>2</v>
+      </c>
+      <c r="S59" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="T59" s="1" t="str">
+        <v>02/15/2019</v>
+      </c>
+      <c r="U59" s="1" t="str">
+        <v>Resecció Major (&gt;= 3 segm)</v>
+      </c>
+      <c r="V59" s="1" t="str">
+        <v>Hepatectomia derecha + reseccion limitada segmento IV</v>
+      </c>
+      <c r="W59" s="1" t="str">
+        <v>Oberta</v>
+      </c>
+      <c r="X59" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="Y59" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="Z59" s="1" t="str">
+        <v>Impressió R0</v>
+      </c>
+      <c r="AA59" s="1">
+        <v>10</v>
+      </c>
+      <c r="AB59" s="1">
+        <v>2</v>
+      </c>
+      <c r="AC59" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AD59" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AE59" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AF59" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AG59" s="1" t="str">
+        <v>0</v>
+      </c>
+      <c r="AH59" s="1">
+        <v>0</v>
+      </c>
+      <c r="AI59" s="1">
+        <v>2</v>
+      </c>
+      <c r="AJ59" s="1">
+        <v>1.3</v>
+      </c>
+      <c r="AK59" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="AL59" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AM59" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AN59" s="2">
+        <v>44522</v>
+      </c>
+      <c r="AO59" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AP59" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AQ59" s="1" t="str">
+        <v>Viu</v>
+      </c>
+      <c r="AR59" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AS59" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AT59" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AU59" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AV59" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AX59" s="1" t="str">
+        <v/>
+      </c>
+      <c r="AY59" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AZ59" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="BA59" s="1">
+        <v>10</v>
+      </c>
+      <c r="BB59" s="2">
+        <v>44610.479952974536</v>
+      </c>
+      <c r="BC59" s="2">
+        <v>43344</v>
+      </c>
+      <c r="BD59" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BE59" s="1" t="str">
+        <v/>
+      </c>
+      <c r="BF59" s="1" t="str">
+        <v/>
+      </c>
+      <c r="BG59" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BJ59" s="1" t="str">
+        <v>hepatectomiaDreta,Segmentectomia1a8</v>
+      </c>
+      <c r="BK59" s="1" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="str">
+        <v>Resecció/ns limitada/es</v>
+      </c>
+      <c r="B60" s="1">
+        <v>1671</v>
+      </c>
+      <c r="C60" s="1" t="str">
+        <v>05/04/2019</v>
+      </c>
+      <c r="D60" s="1" t="str">
+        <v>05/04/2019</v>
+      </c>
+      <c r="E60" s="1" t="str">
+        <v>28/12/2016</v>
+      </c>
+      <c r="F60" s="1" t="str">
+        <v>VIII</v>
+      </c>
+      <c r="G60" s="1">
+        <v>1415</v>
+      </c>
+      <c r="H60" s="1" t="str">
+        <v>Josep M2</v>
+      </c>
+      <c r="I60" s="1" t="str">
+        <v>Balleste2</v>
+      </c>
+      <c r="J60" s="1" t="str">
+        <v>Blasco2</v>
+      </c>
+      <c r="K60" s="1">
+        <v>10207678</v>
+      </c>
+      <c r="L60" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="M60" s="1" t="str">
+        <v>Home</v>
+      </c>
+      <c r="N60" s="1" t="str">
+        <v>75</v>
+      </c>
+      <c r="O60" s="1" t="str">
+        <v>73</v>
+      </c>
+      <c r="P60" s="1">
+        <v>166</v>
+      </c>
+      <c r="Q60" s="1">
+        <v>27</v>
+      </c>
+      <c r="R60" s="1">
+        <v>3</v>
+      </c>
+      <c r="S60" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="T60" s="2">
+        <v>43686</v>
+      </c>
+      <c r="U60" s="1" t="str">
+        <v>Resecció Menor (&lt;3 segm)</v>
+      </c>
+      <c r="V60" s="1" t="str">
+        <v>dues RL segment8</v>
+      </c>
+      <c r="W60" s="1" t="str">
+        <v>Oberta</v>
+      </c>
+      <c r="X60" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="Y60" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="Z60" s="1" t="str">
+        <v>Impressió R1</v>
+      </c>
+      <c r="AA60" s="1">
+        <v>2</v>
+      </c>
+      <c r="AB60" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD60" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AE60" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AF60" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AG60" s="1" t="str">
+        <v>V</v>
+      </c>
+      <c r="AH60" s="1">
+        <v>100</v>
+      </c>
+      <c r="AN60" s="2">
+        <v>43708</v>
+      </c>
+      <c r="AO60" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AP60" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AQ60" s="1" t="str">
+        <v>Mort (lliure malaltia)</v>
+      </c>
+      <c r="AR60" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AS60" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AT60" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AU60" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AV60" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AW60" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AX60" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BA60" s="1">
+        <v>23</v>
+      </c>
+      <c r="BB60" s="2">
+        <v>44610.480130682874</v>
+      </c>
+      <c r="BC60" s="2">
+        <v>42824</v>
+      </c>
+      <c r="BI60" s="2">
+        <v>43708</v>
+      </c>
+      <c r="BJ60" s="1" t="str">
+        <v>no reglada</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="str">
+        <v>Hepatectomia dreta</v>
+      </c>
+      <c r="B61" s="1">
+        <v>1695</v>
+      </c>
+      <c r="C61" s="1" t="str">
+        <v>09/07/2018</v>
+      </c>
+      <c r="D61" s="1" t="str">
+        <v>11/02/2019</v>
+      </c>
+      <c r="E61" s="1" t="str">
+        <v>25/06/2018</v>
+      </c>
+      <c r="F61" s="1" t="str">
+        <v>VII</v>
+      </c>
+      <c r="H61" s="1" t="str">
+        <v>Jordi</v>
+      </c>
+      <c r="I61" s="1" t="str">
+        <v>Morillas2</v>
+      </c>
+      <c r="J61" s="1" t="str">
+        <v>Esteban2</v>
+      </c>
+      <c r="K61" s="1">
+        <v>13296015</v>
+      </c>
+      <c r="L61" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="O61" s="1" t="str">
+        <v>79</v>
+      </c>
+      <c r="P61" s="1">
+        <v>178</v>
+      </c>
+      <c r="Q61" s="1">
+        <v>25</v>
+      </c>
+      <c r="R61" s="1">
+        <v>3</v>
+      </c>
+      <c r="S61" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="T61" s="2">
+        <v>43858</v>
+      </c>
+      <c r="U61" s="1" t="str">
+        <v>Resecció Major (&gt;= 3 segm)</v>
+      </c>
+      <c r="V61" s="1" t="str">
+        <v>hepatectomia dreta</v>
+      </c>
+      <c r="W61" s="1" t="str">
+        <v>Oberta</v>
+      </c>
+      <c r="X61" s="1" t="str">
+        <v>Si, com a primer temps quirúrgic</v>
+      </c>
+      <c r="Y61" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="Z61" s="1" t="str">
+        <v>Impressió R1</v>
+      </c>
+      <c r="AA61" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB61" s="1">
+        <v>3</v>
+      </c>
+      <c r="AC61" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AD61" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AE61" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AF61" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AG61" s="1" t="str">
+        <v>IIIb</v>
+      </c>
+      <c r="AH61" s="1">
+        <v>61</v>
+      </c>
+      <c r="AI61" s="1">
+        <v>1</v>
+      </c>
+      <c r="AJ61" s="1">
+        <v>3</v>
+      </c>
+      <c r="AK61" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL61" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AM61" s="1" t="str">
+        <v>ampliacio quirurgica</v>
+      </c>
+      <c r="AN61" s="2">
+        <v>43983</v>
+      </c>
+      <c r="AO61" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AP61" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AQ61" s="1" t="str">
+        <v>Viu</v>
+      </c>
+      <c r="AR61" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AS61" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AT61" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AU61" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AV61" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AW61" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AX61" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AY61" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AZ61" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BA61" s="1">
+        <v>55</v>
+      </c>
+      <c r="BB61" s="2">
+        <v>44610.48034048611</v>
+      </c>
+      <c r="BC61" s="2">
+        <v>43446</v>
+      </c>
+      <c r="BD61" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BG61" s="1" t="str">
+        <v>oclusió, peritonitis fecaoidea</v>
+      </c>
+      <c r="BH61" s="1">
+        <v>2</v>
+      </c>
+      <c r="BJ61" s="1" t="str">
+        <v>hepatectomiaDreta</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="1" t="str">
+        <v>Hepatectomia dreta</v>
+      </c>
+      <c r="B62" s="1">
+        <v>1695</v>
+      </c>
+      <c r="C62" s="1" t="str">
+        <v>09/07/2018</v>
+      </c>
+      <c r="D62" s="1" t="str">
+        <v>11/02/2019</v>
+      </c>
+      <c r="E62" s="1" t="str">
+        <v>25/06/2018</v>
+      </c>
+      <c r="F62" s="1" t="str">
+        <v>VII</v>
+      </c>
+      <c r="H62" s="1" t="str">
+        <v>Jordi</v>
+      </c>
+      <c r="I62" s="1" t="str">
+        <v>Morillas2</v>
+      </c>
+      <c r="J62" s="1" t="str">
+        <v>Esteban2</v>
+      </c>
+      <c r="K62" s="1">
+        <v>13296015</v>
+      </c>
+      <c r="L62" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="O62" s="1" t="str">
+        <v>79</v>
+      </c>
+      <c r="P62" s="1">
+        <v>178</v>
+      </c>
+      <c r="Q62" s="1">
+        <v>25</v>
+      </c>
+      <c r="R62" s="1">
+        <v>3</v>
+      </c>
+      <c r="S62" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="T62" s="2">
+        <v>43858</v>
+      </c>
+      <c r="U62" s="1" t="str">
+        <v>Resecció Major (&gt;= 3 segm)</v>
+      </c>
+      <c r="V62" s="1" t="str">
+        <v>hepatectomia dreta</v>
+      </c>
+      <c r="W62" s="1" t="str">
+        <v>Oberta</v>
+      </c>
+      <c r="X62" s="1" t="str">
+        <v>Si, com a primer temps quirúrgic</v>
+      </c>
+      <c r="Y62" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="Z62" s="1" t="str">
+        <v>Impressió R1</v>
+      </c>
+      <c r="AA62" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB62" s="1">
+        <v>3</v>
+      </c>
+      <c r="AC62" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AD62" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AE62" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AF62" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AG62" s="1" t="str">
+        <v>IIIb</v>
+      </c>
+      <c r="AH62" s="1">
+        <v>61</v>
+      </c>
+      <c r="AI62" s="1">
+        <v>1</v>
+      </c>
+      <c r="AJ62" s="1">
+        <v>3</v>
+      </c>
+      <c r="AK62" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL62" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AM62" s="1" t="str">
+        <v>ampliacio quirurgica</v>
+      </c>
+      <c r="AN62" s="2">
+        <v>43983</v>
+      </c>
+      <c r="AO62" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AP62" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AQ62" s="1" t="str">
+        <v>Viu</v>
+      </c>
+      <c r="AR62" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AS62" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AT62" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AU62" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AV62" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AW62" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AX62" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AY62" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AZ62" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BA62" s="1">
+        <v>55</v>
+      </c>
+      <c r="BB62" s="2">
+        <v>44610.49999402778</v>
+      </c>
+      <c r="BC62" s="2">
+        <v>43446</v>
+      </c>
+      <c r="BD62" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BG62" s="1" t="str">
+        <v>oclusió, peritonitis fecaoidea</v>
+      </c>
+      <c r="BH62" s="1">
+        <v>2</v>
+      </c>
+      <c r="BJ62" s="1" t="str">
+        <v>hepatectomiaDreta</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="str">
+        <v>Hepatectomia dreta</v>
+      </c>
+      <c r="B63" s="1">
+        <v>1695</v>
+      </c>
+      <c r="C63" s="1" t="str">
+        <v>09/07/2018</v>
+      </c>
+      <c r="D63" s="1" t="str">
+        <v>11/02/2019</v>
+      </c>
+      <c r="E63" s="1" t="str">
+        <v>25/06/2018</v>
+      </c>
+      <c r="F63" s="1" t="str">
+        <v>VII</v>
+      </c>
+      <c r="H63" s="1" t="str">
+        <v>Jordi</v>
+      </c>
+      <c r="I63" s="1" t="str">
+        <v>Morillas2</v>
+      </c>
+      <c r="J63" s="1" t="str">
+        <v>Esteban2</v>
+      </c>
+      <c r="K63" s="1">
+        <v>13296015</v>
+      </c>
+      <c r="L63" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="O63" s="1" t="str">
+        <v>79</v>
+      </c>
+      <c r="P63" s="1">
+        <v>178</v>
+      </c>
+      <c r="Q63" s="1">
+        <v>25</v>
+      </c>
+      <c r="R63" s="1">
+        <v>3</v>
+      </c>
+      <c r="S63" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="T63" s="2">
+        <v>43858</v>
+      </c>
+      <c r="U63" s="1" t="str">
+        <v>Resecció Major (&gt;= 3 segm)</v>
+      </c>
+      <c r="V63" s="1" t="str">
+        <v>hepatectomia dreta</v>
+      </c>
+      <c r="W63" s="1" t="str">
+        <v>Oberta</v>
+      </c>
+      <c r="X63" s="1" t="str">
+        <v>Si, com a primer temps quirúrgic</v>
+      </c>
+      <c r="Y63" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="Z63" s="1" t="str">
+        <v>Impressió R1</v>
+      </c>
+      <c r="AA63" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB63" s="1">
+        <v>3</v>
+      </c>
+      <c r="AC63" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AD63" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AE63" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AF63" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AG63" s="1" t="str">
+        <v>IIIb</v>
+      </c>
+      <c r="AH63" s="1">
+        <v>61</v>
+      </c>
+      <c r="AI63" s="1">
+        <v>1</v>
+      </c>
+      <c r="AJ63" s="1">
+        <v>3</v>
+      </c>
+      <c r="AK63" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL63" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AM63" s="1" t="str">
+        <v>ampliacio quirurgica</v>
+      </c>
+      <c r="AN63" s="2">
+        <v>43983</v>
+      </c>
+      <c r="AO63" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AP63" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AQ63" s="1" t="str">
+        <v>Viu</v>
+      </c>
+      <c r="AR63" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AS63" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AT63" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AU63" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AV63" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AW63" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AX63" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AY63" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AZ63" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BA63" s="1">
+        <v>55</v>
+      </c>
+      <c r="BB63" s="2">
+        <v>44610.504006944444</v>
+      </c>
+      <c r="BC63" s="2">
+        <v>43446</v>
+      </c>
+      <c r="BD63" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BG63" s="1" t="str">
+        <v>oclusió, peritonitis fecaoidea</v>
+      </c>
+      <c r="BH63" s="1">
+        <v>2</v>
+      </c>
+      <c r="BJ63" s="1" t="str">
+        <v>hepatectomiaDreta</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:BJ54"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:BK63"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
complete register for QA
</commit_message>
<xml_diff>
--- a/register/completedRegister.xlsx
+++ b/register/completedRegister.xlsx
@@ -379,7 +379,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BT18"/>
+  <dimension ref="A1:BT21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3132,9 +3132,519 @@
         <v>44610.893191875</v>
       </c>
     </row>
+    <row r="19">
+      <c r="Q19" s="1" t="str">
+        <v>Segmentectomia o Bisegmentectomia</v>
+      </c>
+      <c r="R19" s="1" t="str">
+        <v>bisegmentectomia 6/7</v>
+      </c>
+      <c r="S19" s="1" t="str">
+        <v>Bisegmentectomia6i7</v>
+      </c>
+      <c r="T19" s="1">
+        <v>1703</v>
+      </c>
+      <c r="U19" s="1" t="str">
+        <v>13/12/2019</v>
+      </c>
+      <c r="V19" s="1" t="str">
+        <v>13/12/2019</v>
+      </c>
+      <c r="W19" s="1" t="str">
+        <v>10/12/2019</v>
+      </c>
+      <c r="X19" s="1" t="str">
+        <v>VIII,V</v>
+      </c>
+      <c r="Y19" s="1">
+        <v>1555</v>
+      </c>
+      <c r="Z19" s="1" t="str">
+        <v>Teresa</v>
+      </c>
+      <c r="AA19" s="1" t="str">
+        <v>Asensio</v>
+      </c>
+      <c r="AB19" s="1" t="str">
+        <v>Navarro</v>
+      </c>
+      <c r="AC19" s="1">
+        <v>11396316</v>
+      </c>
+      <c r="AD19" s="2">
+        <v>43900</v>
+      </c>
+      <c r="AE19" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AF19" s="1" t="str">
+        <v>Dona</v>
+      </c>
+      <c r="AG19" s="1" t="str">
+        <v>68</v>
+      </c>
+      <c r="AH19" s="1" t="str">
+        <v>68</v>
+      </c>
+      <c r="AI19" s="1">
+        <v>159</v>
+      </c>
+      <c r="AJ19" s="1">
+        <v>27</v>
+      </c>
+      <c r="AK19" s="1">
+        <v>2</v>
+      </c>
+      <c r="AL19" s="2">
+        <v>43747</v>
+      </c>
+      <c r="AM19" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AN19" s="1" t="str">
+        <v>Resecció Menor (&lt;3 segm)</v>
+      </c>
+      <c r="AO19" s="1" t="str">
+        <v>1er temps (mobilització)</v>
+      </c>
+      <c r="AP19" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AQ19" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AR19" s="1" t="str">
+        <v>Impressió R0</v>
+      </c>
+      <c r="AS19" s="1">
+        <v>1</v>
+      </c>
+      <c r="AT19" s="1">
+        <v>1.8</v>
+      </c>
+      <c r="AU19" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AV19" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AW19" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AX19" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AY19" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AZ19" s="1" t="str">
+        <v>0</v>
+      </c>
+      <c r="BA19" s="1">
+        <v>0</v>
+      </c>
+      <c r="BB19" s="1">
+        <v>1</v>
+      </c>
+      <c r="BC19" s="1">
+        <v>1</v>
+      </c>
+      <c r="BD19" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="BE19" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BF19" s="2">
+        <v>44557</v>
+      </c>
+      <c r="BG19" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BH19" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BI19" s="1" t="str">
+        <v>Viu</v>
+      </c>
+      <c r="BJ19" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BK19" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BL19" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BM19" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BN19" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BO19" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BP19" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BQ19" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BR19" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BS19" s="1">
+        <v>6</v>
+      </c>
+      <c r="BT19" s="2">
+        <v>44611.78876434028</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="Q20" s="1" t="str">
+        <v>Segmentectomia o Bisegmentectomia</v>
+      </c>
+      <c r="R20" s="1" t="str">
+        <v>bisegmentectomia 6/7</v>
+      </c>
+      <c r="S20" s="1" t="str">
+        <v>Bisegmentectomia6i7</v>
+      </c>
+      <c r="T20" s="1">
+        <v>1703</v>
+      </c>
+      <c r="U20" s="1" t="str">
+        <v>13/12/2019</v>
+      </c>
+      <c r="V20" s="1" t="str">
+        <v>13/12/2019</v>
+      </c>
+      <c r="W20" s="1" t="str">
+        <v>10/12/2019</v>
+      </c>
+      <c r="X20" s="1" t="str">
+        <v>VIII,V</v>
+      </c>
+      <c r="Y20" s="1">
+        <v>1555</v>
+      </c>
+      <c r="Z20" s="1" t="str">
+        <v>Teresa</v>
+      </c>
+      <c r="AA20" s="1" t="str">
+        <v>Asensio</v>
+      </c>
+      <c r="AB20" s="1" t="str">
+        <v>Navarro</v>
+      </c>
+      <c r="AC20" s="1">
+        <v>11396316</v>
+      </c>
+      <c r="AD20" s="2">
+        <v>43900</v>
+      </c>
+      <c r="AE20" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AF20" s="1" t="str">
+        <v>Dona</v>
+      </c>
+      <c r="AG20" s="1" t="str">
+        <v>68</v>
+      </c>
+      <c r="AH20" s="1" t="str">
+        <v>68</v>
+      </c>
+      <c r="AI20" s="1">
+        <v>159</v>
+      </c>
+      <c r="AJ20" s="1">
+        <v>27</v>
+      </c>
+      <c r="AK20" s="1">
+        <v>2</v>
+      </c>
+      <c r="AL20" s="2">
+        <v>43747</v>
+      </c>
+      <c r="AM20" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AN20" s="1" t="str">
+        <v>Resecció Menor (&lt;3 segm)</v>
+      </c>
+      <c r="AO20" s="1" t="str">
+        <v>1er temps (mobilització)</v>
+      </c>
+      <c r="AP20" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AQ20" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AR20" s="1" t="str">
+        <v>Impressió R0</v>
+      </c>
+      <c r="AS20" s="1">
+        <v>1</v>
+      </c>
+      <c r="AT20" s="1">
+        <v>1.8</v>
+      </c>
+      <c r="AU20" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AV20" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AW20" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AX20" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AY20" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AZ20" s="1" t="str">
+        <v>0</v>
+      </c>
+      <c r="BA20" s="1">
+        <v>0</v>
+      </c>
+      <c r="BB20" s="1">
+        <v>1</v>
+      </c>
+      <c r="BC20" s="1">
+        <v>1</v>
+      </c>
+      <c r="BD20" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="BE20" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BF20" s="2">
+        <v>44557</v>
+      </c>
+      <c r="BG20" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BH20" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BI20" s="1" t="str">
+        <v>Viu</v>
+      </c>
+      <c r="BJ20" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BK20" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BL20" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BM20" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BN20" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BO20" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BP20" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BQ20" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BR20" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BS20" s="1">
+        <v>6</v>
+      </c>
+      <c r="BT20" s="2">
+        <v>44611.79149173611</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="Q21" s="1" t="str">
+        <v>Segmentectomia o Bisegmentectomia</v>
+      </c>
+      <c r="R21" s="1" t="str">
+        <v>bisegmentectomia 6/7</v>
+      </c>
+      <c r="S21" s="1" t="str">
+        <v>Bisegmentectomia6i7</v>
+      </c>
+      <c r="T21" s="1">
+        <v>1703</v>
+      </c>
+      <c r="U21" s="1" t="str">
+        <v>13/12/2019</v>
+      </c>
+      <c r="V21" s="1" t="str">
+        <v>13/12/2019</v>
+      </c>
+      <c r="W21" s="1" t="str">
+        <v>10/12/2019</v>
+      </c>
+      <c r="X21" s="1" t="str">
+        <v>VIII,V</v>
+      </c>
+      <c r="Y21" s="1">
+        <v>1555</v>
+      </c>
+      <c r="Z21" s="1" t="str">
+        <v>Teresa</v>
+      </c>
+      <c r="AA21" s="1" t="str">
+        <v>Asensio</v>
+      </c>
+      <c r="AB21" s="1" t="str">
+        <v>Navarro</v>
+      </c>
+      <c r="AC21" s="1">
+        <v>11396316</v>
+      </c>
+      <c r="AD21" s="2">
+        <v>43900</v>
+      </c>
+      <c r="AE21" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AF21" s="1" t="str">
+        <v>Dona</v>
+      </c>
+      <c r="AG21" s="1" t="str">
+        <v>68</v>
+      </c>
+      <c r="AH21" s="1" t="str">
+        <v>68</v>
+      </c>
+      <c r="AI21" s="1">
+        <v>159</v>
+      </c>
+      <c r="AJ21" s="1">
+        <v>27</v>
+      </c>
+      <c r="AK21" s="1">
+        <v>2</v>
+      </c>
+      <c r="AL21" s="2">
+        <v>43747</v>
+      </c>
+      <c r="AM21" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AN21" s="1" t="str">
+        <v>Resecció Menor (&lt;3 segm)</v>
+      </c>
+      <c r="AO21" s="1" t="str">
+        <v>1er temps (mobilització)</v>
+      </c>
+      <c r="AP21" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AQ21" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AR21" s="1" t="str">
+        <v>Impressió R0</v>
+      </c>
+      <c r="AS21" s="1">
+        <v>1</v>
+      </c>
+      <c r="AT21" s="1">
+        <v>1.8</v>
+      </c>
+      <c r="AU21" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AV21" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AW21" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AX21" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AY21" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AZ21" s="1" t="str">
+        <v>0</v>
+      </c>
+      <c r="BA21" s="1">
+        <v>0</v>
+      </c>
+      <c r="BB21" s="1">
+        <v>1</v>
+      </c>
+      <c r="BC21" s="1">
+        <v>1</v>
+      </c>
+      <c r="BD21" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="BE21" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BF21" s="2">
+        <v>44557</v>
+      </c>
+      <c r="BG21" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BH21" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BI21" s="1" t="str">
+        <v>Viu</v>
+      </c>
+      <c r="BJ21" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BK21" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BL21" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BM21" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BN21" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BO21" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BP21" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BQ21" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BR21" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BS21" s="1">
+        <v>6</v>
+      </c>
+      <c r="BT21" s="2">
+        <v>44611.79204508102</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:BT18"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:BT21"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add command line arg for check values
</commit_message>
<xml_diff>
--- a/register/completedRegister.xlsx
+++ b/register/completedRegister.xlsx
@@ -379,7 +379,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BT34"/>
+  <dimension ref="A1:BT36"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -5852,9 +5852,349 @@
         <v>44611.819072962964</v>
       </c>
     </row>
+    <row r="35">
+      <c r="Q35" s="1" t="str">
+        <v>Segmentectomia o Bisegmentectomia</v>
+      </c>
+      <c r="R35" s="1" t="str">
+        <v>bisegmentectomia 6/7</v>
+      </c>
+      <c r="S35" s="1" t="str">
+        <v>Bisegmentectomia6i7</v>
+      </c>
+      <c r="T35" s="1">
+        <v>1703</v>
+      </c>
+      <c r="U35" s="1" t="str">
+        <v>13/12/2019</v>
+      </c>
+      <c r="V35" s="1" t="str">
+        <v>13/12/2019</v>
+      </c>
+      <c r="W35" s="1" t="str">
+        <v>10/12/2019</v>
+      </c>
+      <c r="X35" s="1" t="str">
+        <v>VIII,V</v>
+      </c>
+      <c r="Y35" s="1">
+        <v>1555</v>
+      </c>
+      <c r="Z35" s="1" t="str">
+        <v>Teresa</v>
+      </c>
+      <c r="AA35" s="1" t="str">
+        <v>Asensio</v>
+      </c>
+      <c r="AB35" s="1" t="str">
+        <v>Navarro</v>
+      </c>
+      <c r="AC35" s="1">
+        <v>11396316</v>
+      </c>
+      <c r="AD35" s="2">
+        <v>43900</v>
+      </c>
+      <c r="AE35" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AF35" s="1" t="str">
+        <v>Dona</v>
+      </c>
+      <c r="AG35" s="1" t="str">
+        <v>68</v>
+      </c>
+      <c r="AH35" s="1" t="str">
+        <v>68</v>
+      </c>
+      <c r="AI35" s="1">
+        <v>159</v>
+      </c>
+      <c r="AJ35" s="1">
+        <v>27</v>
+      </c>
+      <c r="AK35" s="1">
+        <v>2</v>
+      </c>
+      <c r="AL35" s="2">
+        <v>43747</v>
+      </c>
+      <c r="AM35" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AN35" s="1" t="str">
+        <v>Resecció Menor (&lt;3 segm)</v>
+      </c>
+      <c r="AO35" s="1" t="str">
+        <v>1er temps (mobilització)</v>
+      </c>
+      <c r="AP35" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AQ35" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AR35" s="1" t="str">
+        <v>Impressió R0</v>
+      </c>
+      <c r="AS35" s="1">
+        <v>1</v>
+      </c>
+      <c r="AT35" s="1">
+        <v>1.8</v>
+      </c>
+      <c r="AU35" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AV35" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AW35" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AX35" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AY35" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AZ35" s="1" t="str">
+        <v>0</v>
+      </c>
+      <c r="BA35" s="1">
+        <v>0</v>
+      </c>
+      <c r="BB35" s="1">
+        <v>1</v>
+      </c>
+      <c r="BC35" s="1">
+        <v>1</v>
+      </c>
+      <c r="BD35" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="BE35" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BF35" s="2">
+        <v>44557</v>
+      </c>
+      <c r="BG35" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BH35" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BI35" s="1" t="str">
+        <v>Viu</v>
+      </c>
+      <c r="BJ35" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BK35" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BL35" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BM35" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BN35" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BO35" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BP35" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BQ35" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BR35" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BS35" s="1">
+        <v>6</v>
+      </c>
+      <c r="BT35" s="2">
+        <v>44611.82183226852</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="Q36" s="1" t="str">
+        <v>Segmentectomia o Bisegmentectomia</v>
+      </c>
+      <c r="R36" s="1" t="str">
+        <v>bisegmentectomia 6/7</v>
+      </c>
+      <c r="S36" s="1" t="str">
+        <v>Bisegmentectomia6i7</v>
+      </c>
+      <c r="T36" s="1">
+        <v>1703</v>
+      </c>
+      <c r="U36" s="1" t="str">
+        <v>13/12/2019</v>
+      </c>
+      <c r="V36" s="1" t="str">
+        <v>13/12/2019</v>
+      </c>
+      <c r="W36" s="1" t="str">
+        <v>10/12/2019</v>
+      </c>
+      <c r="X36" s="1" t="str">
+        <v>VIII,V</v>
+      </c>
+      <c r="Y36" s="1">
+        <v>1555</v>
+      </c>
+      <c r="Z36" s="1" t="str">
+        <v>Teresa</v>
+      </c>
+      <c r="AA36" s="1" t="str">
+        <v>Asensio</v>
+      </c>
+      <c r="AB36" s="1" t="str">
+        <v>Navarro</v>
+      </c>
+      <c r="AC36" s="1">
+        <v>11396316</v>
+      </c>
+      <c r="AD36" s="2">
+        <v>43900</v>
+      </c>
+      <c r="AE36" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AF36" s="1" t="str">
+        <v>Dona</v>
+      </c>
+      <c r="AG36" s="1" t="str">
+        <v>68</v>
+      </c>
+      <c r="AH36" s="1" t="str">
+        <v>68</v>
+      </c>
+      <c r="AI36" s="1">
+        <v>159</v>
+      </c>
+      <c r="AJ36" s="1">
+        <v>27</v>
+      </c>
+      <c r="AK36" s="1">
+        <v>2</v>
+      </c>
+      <c r="AL36" s="2">
+        <v>43747</v>
+      </c>
+      <c r="AM36" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AN36" s="1" t="str">
+        <v>Resecció Menor (&lt;3 segm)</v>
+      </c>
+      <c r="AO36" s="1" t="str">
+        <v>1er temps (mobilització)</v>
+      </c>
+      <c r="AP36" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AQ36" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AR36" s="1" t="str">
+        <v>Impressió R0</v>
+      </c>
+      <c r="AS36" s="1">
+        <v>1</v>
+      </c>
+      <c r="AT36" s="1">
+        <v>1.8</v>
+      </c>
+      <c r="AU36" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AV36" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AW36" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AX36" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AY36" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AZ36" s="1" t="str">
+        <v>0</v>
+      </c>
+      <c r="BA36" s="1">
+        <v>0</v>
+      </c>
+      <c r="BB36" s="1">
+        <v>1</v>
+      </c>
+      <c r="BC36" s="1">
+        <v>1</v>
+      </c>
+      <c r="BD36" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="BE36" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BF36" s="2">
+        <v>44557</v>
+      </c>
+      <c r="BG36" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BH36" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BI36" s="1" t="str">
+        <v>Viu</v>
+      </c>
+      <c r="BJ36" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BK36" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BL36" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BM36" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BN36" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BO36" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BP36" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BQ36" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BR36" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BS36" s="1">
+        <v>6</v>
+      </c>
+      <c r="BT36" s="2">
+        <v>44611.82285181713</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:BT34"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:BT36"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
solve dist marge resecció
</commit_message>
<xml_diff>
--- a/register/completedRegister.xlsx
+++ b/register/completedRegister.xlsx
@@ -379,7 +379,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BF6"/>
+  <dimension ref="A1:BF13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1392,9 +1392,1172 @@
         <v>43721</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" s="1" t="str">
+        <v>Segmentectomia o Bisegmentectomia</v>
+      </c>
+      <c r="B7" s="1" t="str">
+        <v>segmentectomia 5</v>
+      </c>
+      <c r="C7" s="1" t="str">
+        <v>Segmentectomia1a8</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1676</v>
+      </c>
+      <c r="E7" s="1" t="str">
+        <v>19/07/2019</v>
+      </c>
+      <c r="F7" s="1" t="str">
+        <v>19/07/2019</v>
+      </c>
+      <c r="G7" s="1" t="str">
+        <v>26/6/19</v>
+      </c>
+      <c r="H7" s="1" t="str">
+        <v>V,IV</v>
+      </c>
+      <c r="I7" s="1">
+        <v>1534</v>
+      </c>
+      <c r="J7" s="1" t="str">
+        <v>Francesc</v>
+      </c>
+      <c r="K7" s="1" t="str">
+        <v>Dolera</v>
+      </c>
+      <c r="L7" s="1" t="str">
+        <v>bernal</v>
+      </c>
+      <c r="M7" s="1">
+        <v>12817360</v>
+      </c>
+      <c r="N7" s="2">
+        <v>43725</v>
+      </c>
+      <c r="O7" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="P7" s="1" t="str">
+        <v>Home</v>
+      </c>
+      <c r="Q7" s="1" t="str">
+        <v>60</v>
+      </c>
+      <c r="R7" s="1" t="str">
+        <v>80</v>
+      </c>
+      <c r="S7" s="1">
+        <v>170</v>
+      </c>
+      <c r="T7" s="1">
+        <v>26</v>
+      </c>
+      <c r="U7" s="1">
+        <v>2</v>
+      </c>
+      <c r="V7" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="W7" s="1" t="str">
+        <v>Resecció Menor (&lt;3 segm)</v>
+      </c>
+      <c r="X7" s="1" t="str">
+        <v>Oberta</v>
+      </c>
+      <c r="Y7" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="Z7" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AA7" s="1" t="str">
+        <v>Impressió R0</v>
+      </c>
+      <c r="AB7" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC7" s="1">
+        <v>2</v>
+      </c>
+      <c r="AD7" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AE7" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AF7" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AG7" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AH7" s="1" t="str">
+        <v>0</v>
+      </c>
+      <c r="AI7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AJ7" s="1">
+        <v>1</v>
+      </c>
+      <c r="AK7" s="1">
+        <v>5</v>
+      </c>
+      <c r="AL7" s="1">
+        <v>1</v>
+      </c>
+      <c r="AM7" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AO7" s="2">
+        <v>44421</v>
+      </c>
+      <c r="AP7" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AQ7" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AR7" s="1" t="str">
+        <v>Viu</v>
+      </c>
+      <c r="AS7" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AT7" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AU7" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AV7" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AW7" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AX7" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AY7" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BB7" s="1">
+        <v>6</v>
+      </c>
+      <c r="BC7" s="2">
+        <v>44614.35327677083</v>
+      </c>
+      <c r="BD7" s="2">
+        <v>43175</v>
+      </c>
+      <c r="BE7" s="1" t="str">
+        <v>No</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="str">
+        <v>Segmentectomia o Bisegmentectomia</v>
+      </c>
+      <c r="B8" s="1" t="str">
+        <v>segmentectomia 5</v>
+      </c>
+      <c r="C8" s="1" t="str">
+        <v>Segmentectomia1a8</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1676</v>
+      </c>
+      <c r="E8" s="1" t="str">
+        <v>19/07/2019</v>
+      </c>
+      <c r="F8" s="1" t="str">
+        <v>19/07/2019</v>
+      </c>
+      <c r="G8" s="1" t="str">
+        <v>26/6/19</v>
+      </c>
+      <c r="H8" s="1" t="str">
+        <v>V,IV</v>
+      </c>
+      <c r="I8" s="1">
+        <v>1534</v>
+      </c>
+      <c r="J8" s="1" t="str">
+        <v>Francesc</v>
+      </c>
+      <c r="K8" s="1" t="str">
+        <v>Dolera</v>
+      </c>
+      <c r="L8" s="1" t="str">
+        <v>bernal</v>
+      </c>
+      <c r="M8" s="1">
+        <v>12817360</v>
+      </c>
+      <c r="N8" s="2">
+        <v>43725</v>
+      </c>
+      <c r="O8" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="P8" s="1" t="str">
+        <v>Home</v>
+      </c>
+      <c r="Q8" s="1" t="str">
+        <v>60</v>
+      </c>
+      <c r="R8" s="1" t="str">
+        <v>80</v>
+      </c>
+      <c r="S8" s="1">
+        <v>170</v>
+      </c>
+      <c r="T8" s="1">
+        <v>26</v>
+      </c>
+      <c r="U8" s="1">
+        <v>2</v>
+      </c>
+      <c r="V8" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="W8" s="1" t="str">
+        <v>Resecció Menor (&lt;3 segm)</v>
+      </c>
+      <c r="X8" s="1" t="str">
+        <v>Oberta</v>
+      </c>
+      <c r="Y8" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="Z8" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AA8" s="1" t="str">
+        <v>Impressió R0</v>
+      </c>
+      <c r="AB8" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC8" s="1">
+        <v>2</v>
+      </c>
+      <c r="AD8" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AE8" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AF8" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AG8" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AH8" s="1" t="str">
+        <v>0</v>
+      </c>
+      <c r="AI8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AJ8" s="1">
+        <v>1</v>
+      </c>
+      <c r="AK8" s="1">
+        <v>5</v>
+      </c>
+      <c r="AL8" s="1">
+        <v>1</v>
+      </c>
+      <c r="AM8" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AO8" s="2">
+        <v>44421</v>
+      </c>
+      <c r="AP8" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AQ8" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AR8" s="1" t="str">
+        <v>Viu</v>
+      </c>
+      <c r="AS8" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AT8" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AU8" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AV8" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AW8" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AX8" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AY8" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="BB8" s="1">
+        <v>6</v>
+      </c>
+      <c r="BC8" s="2">
+        <v>44614.35377028935</v>
+      </c>
+      <c r="BD8" s="2">
+        <v>43175</v>
+      </c>
+      <c r="BE8" s="1" t="str">
+        <v>No</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="str">
+        <v>Segmentectomia o Bisegmentectomia</v>
+      </c>
+      <c r="B9" s="1" t="str">
+        <v>segmentect 5 i 2 RL</v>
+      </c>
+      <c r="C9" s="1" t="str">
+        <v>Segmentectomia1a8</v>
+      </c>
+      <c r="D9" s="1">
+        <v>1694</v>
+      </c>
+      <c r="E9" s="1" t="str">
+        <v>18/10/2019</v>
+      </c>
+      <c r="F9" s="1" t="str">
+        <v>18/10/2019</v>
+      </c>
+      <c r="G9" s="1" t="str">
+        <v>16/07/2019</v>
+      </c>
+      <c r="H9" s="1" t="str">
+        <v>II,V,VIII,VII</v>
+      </c>
+      <c r="I9" s="1">
+        <v>1548</v>
+      </c>
+      <c r="J9" s="1" t="str">
+        <v>Fco jesus</v>
+      </c>
+      <c r="K9" s="1" t="str">
+        <v>Herrera</v>
+      </c>
+      <c r="L9" s="1" t="str">
+        <v>Exposito</v>
+      </c>
+      <c r="M9" s="1">
+        <v>13611095</v>
+      </c>
+      <c r="N9" s="2">
+        <v>43846</v>
+      </c>
+      <c r="O9" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="P9" s="1" t="str">
+        <v>Home</v>
+      </c>
+      <c r="Q9" s="1" t="str">
+        <v>61</v>
+      </c>
+      <c r="R9" s="1" t="str">
+        <v>76</v>
+      </c>
+      <c r="S9" s="1">
+        <v>175</v>
+      </c>
+      <c r="T9" s="1">
+        <v>25</v>
+      </c>
+      <c r="U9" s="1">
+        <v>2</v>
+      </c>
+      <c r="V9" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="W9" s="1" t="str">
+        <v>Resecció Menor (&lt;3 segm)</v>
+      </c>
+      <c r="X9" s="1" t="str">
+        <v>1er temps (mobilització)</v>
+      </c>
+      <c r="Y9" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="Z9" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AA9" s="1" t="str">
+        <v>Impressió R1</v>
+      </c>
+      <c r="AB9" s="1">
+        <v>3</v>
+      </c>
+      <c r="AC9" s="1">
+        <v>2</v>
+      </c>
+      <c r="AD9" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AE9" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AF9" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AG9" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AH9" s="1" t="str">
+        <v>IIIa</v>
+      </c>
+      <c r="AJ9" s="1">
+        <v>3</v>
+      </c>
+      <c r="AK9" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="AL9" s="1">
+        <v>0</v>
+      </c>
+      <c r="AM9" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AN9" s="1" t="str">
+        <v>ampli quirúgica i Aquamantis</v>
+      </c>
+      <c r="AO9" s="2">
+        <v>44243</v>
+      </c>
+      <c r="AP9" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AQ9" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AR9" s="1" t="str">
+        <v>Viu</v>
+      </c>
+      <c r="AS9" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AT9" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AU9" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AV9" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AW9" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AX9" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AY9" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AZ9" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="BA9" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="BB9" s="1">
+        <v>6</v>
+      </c>
+      <c r="BC9" s="2">
+        <v>44614.35471002315</v>
+      </c>
+      <c r="BD9" s="2">
+        <v>43721</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="str">
+        <v>Segmentectomia o Bisegmentectomia</v>
+      </c>
+      <c r="B10" s="1" t="str">
+        <v>segmentect 5 i 2 RL</v>
+      </c>
+      <c r="C10" s="1" t="str">
+        <v>Segmentectomia1a8</v>
+      </c>
+      <c r="D10" s="1">
+        <v>1694</v>
+      </c>
+      <c r="E10" s="1" t="str">
+        <v>18/10/2019</v>
+      </c>
+      <c r="F10" s="1" t="str">
+        <v>18/10/2019</v>
+      </c>
+      <c r="G10" s="1" t="str">
+        <v>16/07/2019</v>
+      </c>
+      <c r="H10" s="1" t="str">
+        <v>II,V,VIII,VII</v>
+      </c>
+      <c r="I10" s="1">
+        <v>1548</v>
+      </c>
+      <c r="J10" s="1" t="str">
+        <v>Fco jesus</v>
+      </c>
+      <c r="K10" s="1" t="str">
+        <v>Herrera</v>
+      </c>
+      <c r="L10" s="1" t="str">
+        <v>Exposito</v>
+      </c>
+      <c r="M10" s="1">
+        <v>13611095</v>
+      </c>
+      <c r="N10" s="2">
+        <v>43846</v>
+      </c>
+      <c r="O10" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="P10" s="1" t="str">
+        <v>Home</v>
+      </c>
+      <c r="Q10" s="1" t="str">
+        <v>61</v>
+      </c>
+      <c r="R10" s="1" t="str">
+        <v>76</v>
+      </c>
+      <c r="S10" s="1">
+        <v>175</v>
+      </c>
+      <c r="T10" s="1">
+        <v>25</v>
+      </c>
+      <c r="U10" s="1">
+        <v>2</v>
+      </c>
+      <c r="V10" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="W10" s="1" t="str">
+        <v>Resecció Menor (&lt;3 segm)</v>
+      </c>
+      <c r="X10" s="1" t="str">
+        <v>1er temps (mobilització)</v>
+      </c>
+      <c r="Y10" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="Z10" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AA10" s="1" t="str">
+        <v>Impressió R1</v>
+      </c>
+      <c r="AB10" s="1">
+        <v>3</v>
+      </c>
+      <c r="AC10" s="1">
+        <v>2</v>
+      </c>
+      <c r="AD10" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AE10" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AF10" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AG10" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AH10" s="1" t="str">
+        <v>IIIa</v>
+      </c>
+      <c r="AJ10" s="1">
+        <v>3</v>
+      </c>
+      <c r="AK10" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="AL10" s="1">
+        <v>0</v>
+      </c>
+      <c r="AM10" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AN10" s="1" t="str">
+        <v>ampli quirúgica i Aquamantis</v>
+      </c>
+      <c r="AO10" s="2">
+        <v>44243</v>
+      </c>
+      <c r="AP10" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AQ10" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AR10" s="1" t="str">
+        <v>Viu</v>
+      </c>
+      <c r="AS10" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AT10" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AU10" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AV10" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AW10" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AX10" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AY10" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AZ10" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="BA10" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="BB10" s="1">
+        <v>6</v>
+      </c>
+      <c r="BC10" s="2">
+        <v>44614.35498545139</v>
+      </c>
+      <c r="BD10" s="2">
+        <v>43721</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="str">
+        <v>Segmentectomia o Bisegmentectomia</v>
+      </c>
+      <c r="B11" s="1" t="str">
+        <v>segmentect 5 i 2 RL</v>
+      </c>
+      <c r="C11" s="1" t="str">
+        <v>Segmentectomia1a8</v>
+      </c>
+      <c r="D11" s="1">
+        <v>1694</v>
+      </c>
+      <c r="E11" s="1" t="str">
+        <v>18/10/2019</v>
+      </c>
+      <c r="F11" s="1" t="str">
+        <v>18/10/2019</v>
+      </c>
+      <c r="G11" s="1" t="str">
+        <v>16/07/2019</v>
+      </c>
+      <c r="H11" s="1" t="str">
+        <v>II,V,VIII,VII</v>
+      </c>
+      <c r="I11" s="1">
+        <v>1548</v>
+      </c>
+      <c r="J11" s="1" t="str">
+        <v>Fco jesus</v>
+      </c>
+      <c r="K11" s="1" t="str">
+        <v>Herrera</v>
+      </c>
+      <c r="L11" s="1" t="str">
+        <v>Exposito</v>
+      </c>
+      <c r="M11" s="1">
+        <v>13611095</v>
+      </c>
+      <c r="N11" s="2">
+        <v>43846</v>
+      </c>
+      <c r="O11" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="P11" s="1" t="str">
+        <v>Home</v>
+      </c>
+      <c r="Q11" s="1" t="str">
+        <v>61</v>
+      </c>
+      <c r="R11" s="1" t="str">
+        <v>76</v>
+      </c>
+      <c r="S11" s="1">
+        <v>175</v>
+      </c>
+      <c r="T11" s="1">
+        <v>25</v>
+      </c>
+      <c r="U11" s="1">
+        <v>2</v>
+      </c>
+      <c r="V11" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="W11" s="1" t="str">
+        <v>Resecció Menor (&lt;3 segm)</v>
+      </c>
+      <c r="X11" s="1" t="str">
+        <v>1er temps (mobilització)</v>
+      </c>
+      <c r="Y11" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="Z11" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AA11" s="1" t="str">
+        <v>Impressió R1</v>
+      </c>
+      <c r="AB11" s="1">
+        <v>3</v>
+      </c>
+      <c r="AC11" s="1">
+        <v>2</v>
+      </c>
+      <c r="AD11" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AE11" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AF11" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AG11" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AH11" s="1" t="str">
+        <v>IIIa</v>
+      </c>
+      <c r="AJ11" s="1">
+        <v>3</v>
+      </c>
+      <c r="AK11" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="AL11" s="1">
+        <v>0</v>
+      </c>
+      <c r="AM11" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AN11" s="1" t="str">
+        <v>ampli quirúgica i Aquamantis</v>
+      </c>
+      <c r="AO11" s="2">
+        <v>44243</v>
+      </c>
+      <c r="AP11" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AQ11" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AR11" s="1" t="str">
+        <v>Viu</v>
+      </c>
+      <c r="AS11" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AT11" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AU11" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AV11" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AW11" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AX11" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AY11" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AZ11" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="BA11" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="BB11" s="1">
+        <v>6</v>
+      </c>
+      <c r="BC11" s="2">
+        <v>44614.35590646991</v>
+      </c>
+      <c r="BD11" s="2">
+        <v>43721</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="str">
+        <v>Segmentectomia o Bisegmentectomia</v>
+      </c>
+      <c r="B12" s="1" t="str">
+        <v>segmentect 5 i 2 RL</v>
+      </c>
+      <c r="C12" s="1" t="str">
+        <v>Segmentectomia1a8</v>
+      </c>
+      <c r="D12" s="1">
+        <v>1694</v>
+      </c>
+      <c r="E12" s="1" t="str">
+        <v>18/10/2019</v>
+      </c>
+      <c r="F12" s="1" t="str">
+        <v>18/10/2019</v>
+      </c>
+      <c r="G12" s="1" t="str">
+        <v>16/07/2019</v>
+      </c>
+      <c r="H12" s="1" t="str">
+        <v>II,V,VIII,VII</v>
+      </c>
+      <c r="I12" s="1">
+        <v>1548</v>
+      </c>
+      <c r="J12" s="1" t="str">
+        <v>Fco jesus</v>
+      </c>
+      <c r="K12" s="1" t="str">
+        <v>Herrera</v>
+      </c>
+      <c r="L12" s="1" t="str">
+        <v>Exposito</v>
+      </c>
+      <c r="M12" s="1">
+        <v>13611095</v>
+      </c>
+      <c r="N12" s="2">
+        <v>43846</v>
+      </c>
+      <c r="O12" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="P12" s="1" t="str">
+        <v>Home</v>
+      </c>
+      <c r="Q12" s="1" t="str">
+        <v>61</v>
+      </c>
+      <c r="R12" s="1" t="str">
+        <v>76</v>
+      </c>
+      <c r="S12" s="1">
+        <v>175</v>
+      </c>
+      <c r="T12" s="1">
+        <v>25</v>
+      </c>
+      <c r="U12" s="1">
+        <v>2</v>
+      </c>
+      <c r="V12" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="W12" s="1" t="str">
+        <v>Resecció Menor (&lt;3 segm)</v>
+      </c>
+      <c r="X12" s="1" t="str">
+        <v>1er temps (mobilització)</v>
+      </c>
+      <c r="Y12" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="Z12" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AA12" s="1" t="str">
+        <v>Impressió R1</v>
+      </c>
+      <c r="AB12" s="1">
+        <v>3</v>
+      </c>
+      <c r="AC12" s="1">
+        <v>2</v>
+      </c>
+      <c r="AD12" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AE12" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AF12" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AG12" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AH12" s="1" t="str">
+        <v>IIIa</v>
+      </c>
+      <c r="AJ12" s="1">
+        <v>3</v>
+      </c>
+      <c r="AK12" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="AL12" s="1">
+        <v>0</v>
+      </c>
+      <c r="AM12" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AN12" s="1" t="str">
+        <v>ampli quirúgica i Aquamantis</v>
+      </c>
+      <c r="AO12" s="2">
+        <v>44243</v>
+      </c>
+      <c r="AP12" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AQ12" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AR12" s="1" t="str">
+        <v>Viu</v>
+      </c>
+      <c r="AS12" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AT12" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AU12" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AV12" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AW12" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AX12" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AY12" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AZ12" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="BA12" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="BB12" s="1">
+        <v>6</v>
+      </c>
+      <c r="BC12" s="2">
+        <v>44614.35669915509</v>
+      </c>
+      <c r="BD12" s="2">
+        <v>43721</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="str">
+        <v>Segmentectomia o Bisegmentectomia</v>
+      </c>
+      <c r="B13" s="1" t="str">
+        <v>segmentect 5 i 2 RL</v>
+      </c>
+      <c r="C13" s="1" t="str">
+        <v>Segmentectomia1a8</v>
+      </c>
+      <c r="D13" s="1">
+        <v>1694</v>
+      </c>
+      <c r="E13" s="1" t="str">
+        <v>18/10/2019</v>
+      </c>
+      <c r="F13" s="1" t="str">
+        <v>18/10/2019</v>
+      </c>
+      <c r="G13" s="1" t="str">
+        <v>16/07/2019</v>
+      </c>
+      <c r="H13" s="1" t="str">
+        <v>II,V,VIII,VII</v>
+      </c>
+      <c r="I13" s="1">
+        <v>1548</v>
+      </c>
+      <c r="J13" s="1" t="str">
+        <v>Fco jesus</v>
+      </c>
+      <c r="K13" s="1" t="str">
+        <v>Herrera</v>
+      </c>
+      <c r="L13" s="1" t="str">
+        <v>Exposito</v>
+      </c>
+      <c r="M13" s="1">
+        <v>13611095</v>
+      </c>
+      <c r="N13" s="2">
+        <v>43846</v>
+      </c>
+      <c r="O13" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="P13" s="1" t="str">
+        <v>Home</v>
+      </c>
+      <c r="Q13" s="1" t="str">
+        <v>61</v>
+      </c>
+      <c r="R13" s="1" t="str">
+        <v>76</v>
+      </c>
+      <c r="S13" s="1">
+        <v>175</v>
+      </c>
+      <c r="T13" s="1">
+        <v>25</v>
+      </c>
+      <c r="U13" s="1">
+        <v>2</v>
+      </c>
+      <c r="V13" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="W13" s="1" t="str">
+        <v>Resecció Menor (&lt;3 segm)</v>
+      </c>
+      <c r="X13" s="1" t="str">
+        <v>1er temps (mobilització)</v>
+      </c>
+      <c r="Y13" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="Z13" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AA13" s="1" t="str">
+        <v>Impressió R1</v>
+      </c>
+      <c r="AB13" s="1">
+        <v>3</v>
+      </c>
+      <c r="AC13" s="1">
+        <v>2</v>
+      </c>
+      <c r="AD13" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AE13" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AF13" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AG13" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AH13" s="1" t="str">
+        <v>IIIa</v>
+      </c>
+      <c r="AJ13" s="1">
+        <v>3</v>
+      </c>
+      <c r="AK13" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="AL13" s="1">
+        <v>0</v>
+      </c>
+      <c r="AM13" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AN13" s="1" t="str">
+        <v>ampli quirúgica i Aquamantis</v>
+      </c>
+      <c r="AO13" s="2">
+        <v>44243</v>
+      </c>
+      <c r="AP13" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AQ13" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AR13" s="1" t="str">
+        <v>Viu</v>
+      </c>
+      <c r="AS13" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AT13" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AU13" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AV13" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AW13" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AX13" s="1" t="str">
+        <v>No</v>
+      </c>
+      <c r="AY13" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="AZ13" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="BA13" s="1" t="str">
+        <v>Si</v>
+      </c>
+      <c r="BB13" s="1">
+        <v>6</v>
+      </c>
+      <c r="BC13" s="2">
+        <v>44614.35753907407</v>
+      </c>
+      <c r="BD13" s="2">
+        <v>43721</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:BF6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:BF13"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>